<commit_message>
update timesheet period december
</commit_message>
<xml_diff>
--- a/12_Period_20_Nov_2024_sd_19_Dec_2024/Timesheet Danamon_Bayu Bagus Bagaswara_December.xlsx
+++ b/12_Period_20_Nov_2024_sd_19_Dec_2024/Timesheet Danamon_Bayu Bagus Bagaswara_December.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bankdanamonindonesia-my.sharepoint.com/personal/v00028684_danamon_co_id/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayub\Projects Bayu\TIMESHEET DANAMON BAYU\12_Period_20_Nov_2024_sd_19_Dec_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{E58959C0-AE5B-42AE-AFC7-9E35B7F9C350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDF3A40D-420E-44A0-9B5C-6199ABB9985F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D657A15-93D2-4F38-9011-F5A6AB9366BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="1" activeTab="1" xr2:uid="{287076C2-500C-4AE4-B01E-3C74A6B599A0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{287076C2-500C-4AE4-B01E-3C74A6B599A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Timesheet_Template (OLD)" sheetId="28" state="hidden" r:id="rId1"/>
@@ -20,24 +20,33 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Timesheet_Template (OLD)'!$A$1:$AL$49</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -52,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="184">
   <si>
     <t>Timesheet Period</t>
   </si>
@@ -265,12 +274,6 @@
   </si>
   <si>
     <t>* = optional</t>
-  </si>
-  <si>
-    <t>Britney</t>
-  </si>
-  <si>
-    <t>Spears</t>
   </si>
   <si>
     <t xml:space="preserve">TIMESHEET GUIDELINE </t>
@@ -700,6 +703,65 @@
   </si>
   <si>
     <t>IT Java Developer</t>
+  </si>
+  <si>
+    <t>Edy Yanto</t>
+  </si>
+  <si>
+    <t>Dody Arya</t>
+  </si>
+  <si>
+    <t>PO.67515</t>
+  </si>
+  <si>
+    <t>Bank Danamon Falatehan</t>
+  </si>
+  <si>
+    <t>Daily IT TFC</t>
+  </si>
+  <si>
+    <t>19-Dec-2024
+Bayu Bagus Bagaswara</t>
+  </si>
+  <si>
+    <t>please drop your signature here
+Dody Arya</t>
+  </si>
+  <si>
+    <t>Added the TestDROIncomeController class as a data connection and test for Income query.</t>
+  </si>
+  <si>
+    <t>Added the TestDROLBABKController class as a data connection and test for LBABK query.</t>
+  </si>
+  <si>
+    <t>Added the TestDROLKPBUController class as a data connection and test for LKPBU query.</t>
+  </si>
+  <si>
+    <t>Create a new API with the /get-dro endpoint in LBABKController and connect it to the LBABKDROService service.</t>
+  </si>
+  <si>
+    <t>Create a new API with the /get-dro endpoint in LKPBUController and connect it to the LKPBUDROService service.</t>
+  </si>
+  <si>
+    <t>Create a new API with the /get-dro endpoint in LKPBUIncomeController and connect it to the LKPBUIncomeDROService service.</t>
+  </si>
+  <si>
+    <t>Create a logic layer LBABKDROService. Create a loadQuery method for query_get_lbabk.sql. Create a connection to the hiport database and map the query result data to variable LBABKDataSource objects.</t>
+  </si>
+  <si>
+    <t>Create a logic layer LKPBUDROService. Create a loadQuery method for query_get_lkpbu.sql. Create a connection to the hiport database and map the query result data to variable LKPBUDataSource objects.</t>
+  </si>
+  <si>
+    <t>Create a logic layer LKPBUIncomeDROService. Create a loadQuery method for query_get_income.sql. Create a connection to the hiport database and map the query result data to variable LKPBUIncome objects.</t>
+  </si>
+  <si>
+    <t>Changed the encapsulation of some methods in the CsvDataMapper utility so that they can be accessed from other classes. Added methods for data parsing such as, checkAndConvertSheetUnitLKPBU, parseSettleDateLBABK, parseSettleDateIncome, getKodeEfekLKPBU, parseToBigDecimalLKPBU, parseToBigDecimalLBABK, parseToBigDecimalIncome.</t>
+  </si>
+  <si>
+    <t>Monitoring generate LKPBU</t>
+  </si>
+  <si>
+    <t>CRF-5094</t>
   </si>
 </sst>
 </file>
@@ -1502,7 +1564,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="204">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1905,6 +1967,9 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2087,6 +2152,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2101,6 +2175,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -2109,20 +2197,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2725,12 +2799,12 @@
       </c>
       <c r="L5" s="78"/>
       <c r="M5" s="78"/>
-      <c r="N5" s="150" t="s">
+      <c r="N5" s="151" t="s">
         <v>11</v>
       </c>
-      <c r="O5" s="150"/>
-      <c r="P5" s="150"/>
-      <c r="Q5" s="150"/>
+      <c r="O5" s="151"/>
+      <c r="P5" s="151"/>
+      <c r="Q5" s="151"/>
     </row>
     <row r="6" spans="1:35" ht="17" x14ac:dyDescent="0.4">
       <c r="A6" s="74" t="s">
@@ -2755,12 +2829,12 @@
       </c>
       <c r="L6" s="87"/>
       <c r="M6" s="76"/>
-      <c r="N6" s="149" t="s">
+      <c r="N6" s="150" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="149"/>
-      <c r="P6" s="149"/>
-      <c r="Q6" s="149"/>
+      <c r="O6" s="150"/>
+      <c r="P6" s="150"/>
+      <c r="Q6" s="150"/>
       <c r="W6"/>
     </row>
     <row r="7" spans="1:35" s="42" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -2783,13 +2857,13 @@
       <c r="Q7" s="76"/>
     </row>
     <row r="9" spans="1:35" ht="17" x14ac:dyDescent="0.35">
-      <c r="A9" s="140" t="s">
+      <c r="A9" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="141" t="s">
+      <c r="B9" s="142" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="140" t="s">
+      <c r="C9" s="141" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="50" t="str">
@@ -2912,7 +2986,7 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="AH9" s="141" t="s">
+      <c r="AH9" s="142" t="s">
         <v>23</v>
       </c>
       <c r="AI9" s="90" t="s">
@@ -2920,9 +2994,9 @@
       </c>
     </row>
     <row r="10" spans="1:35" ht="17" x14ac:dyDescent="0.35">
-      <c r="A10" s="140"/>
-      <c r="B10" s="141"/>
-      <c r="C10" s="140"/>
+      <c r="A10" s="141"/>
+      <c r="B10" s="142"/>
+      <c r="C10" s="141"/>
       <c r="D10" s="51" cm="1">
         <f t="array" ref="D10:AG10">IFERROR(IF(OR((B3-B2+1)&gt;31,B2="",B3=""),"",_xlfn.SEQUENCE(,B3-B2+1,B2)),"")</f>
         <v>45536</v>
@@ -3014,7 +3088,7 @@
       <c r="AG10" s="51">
         <v>45565</v>
       </c>
-      <c r="AH10" s="141"/>
+      <c r="AH10" s="142"/>
       <c r="AI10" s="90"/>
     </row>
     <row r="11" spans="1:35" ht="17" x14ac:dyDescent="0.4">
@@ -3626,11 +3700,11 @@
       <c r="AI21" s="73"/>
     </row>
     <row r="22" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A22" s="142" t="s">
+      <c r="A22" s="143" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="143"/>
-      <c r="C22" s="144"/>
+      <c r="B22" s="144"/>
+      <c r="C22" s="145"/>
       <c r="D22" s="57"/>
       <c r="E22" s="57">
         <v>8</v>
@@ -3674,11 +3748,11 @@
       <c r="AI22" s="73"/>
     </row>
     <row r="23" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A23" s="142" t="s">
+      <c r="A23" s="143" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="143"/>
-      <c r="C23" s="144"/>
+      <c r="B23" s="144"/>
+      <c r="C23" s="145"/>
       <c r="D23" s="57"/>
       <c r="E23" s="57"/>
       <c r="F23" s="57">
@@ -3718,11 +3792,11 @@
       <c r="AI23" s="73"/>
     </row>
     <row r="24" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A24" s="145" t="s">
+      <c r="A24" s="146" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="146"/>
-      <c r="C24" s="147"/>
+      <c r="B24" s="147"/>
+      <c r="C24" s="148"/>
       <c r="D24" s="57"/>
       <c r="E24" s="57"/>
       <c r="F24" s="57"/>
@@ -3762,11 +3836,11 @@
       <c r="AI24" s="73"/>
     </row>
     <row r="25" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A25" s="142" t="s">
+      <c r="A25" s="143" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="143"/>
-      <c r="C25" s="144"/>
+      <c r="B25" s="144"/>
+      <c r="C25" s="145"/>
       <c r="D25" s="57"/>
       <c r="E25" s="57">
         <f t="shared" ref="E25:AB25" si="1">SUM(E11:E20)</f>
@@ -3897,145 +3971,145 @@
         <v>42</v>
       </c>
       <c r="D27" s="4"/>
-      <c r="E27" s="151"/>
-      <c r="F27" s="151"/>
-      <c r="G27" s="151"/>
-      <c r="H27" s="151"/>
-      <c r="I27" s="151"/>
-      <c r="J27" s="151"/>
-      <c r="S27" s="170" t="s">
+      <c r="E27" s="152"/>
+      <c r="F27" s="152"/>
+      <c r="G27" s="152"/>
+      <c r="H27" s="152"/>
+      <c r="I27" s="152"/>
+      <c r="J27" s="152"/>
+      <c r="S27" s="171" t="s">
         <v>43</v>
       </c>
-      <c r="T27" s="171"/>
-      <c r="U27" s="171"/>
-      <c r="V27" s="171"/>
-      <c r="W27" s="171"/>
-      <c r="X27" s="171"/>
-      <c r="Y27" s="171"/>
-      <c r="Z27" s="171"/>
-      <c r="AA27" s="172"/>
-      <c r="AC27" s="178" t="s">
+      <c r="T27" s="172"/>
+      <c r="U27" s="172"/>
+      <c r="V27" s="172"/>
+      <c r="W27" s="172"/>
+      <c r="X27" s="172"/>
+      <c r="Y27" s="172"/>
+      <c r="Z27" s="172"/>
+      <c r="AA27" s="173"/>
+      <c r="AC27" s="179" t="s">
         <v>44</v>
       </c>
-      <c r="AD27" s="179"/>
-      <c r="AE27" s="179"/>
-      <c r="AF27" s="179"/>
-      <c r="AG27" s="179"/>
-      <c r="AH27" s="179"/>
-      <c r="AI27" s="179"/>
-      <c r="AJ27" s="180"/>
+      <c r="AD27" s="180"/>
+      <c r="AE27" s="180"/>
+      <c r="AF27" s="180"/>
+      <c r="AG27" s="180"/>
+      <c r="AH27" s="180"/>
+      <c r="AI27" s="180"/>
+      <c r="AJ27" s="181"/>
     </row>
     <row r="28" spans="1:36" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="69"/>
       <c r="B28" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="151"/>
-      <c r="F28" s="151"/>
-      <c r="G28" s="151"/>
-      <c r="H28" s="151"/>
-      <c r="I28" s="151"/>
-      <c r="J28" s="151"/>
-      <c r="S28" s="161" t="s">
+      <c r="E28" s="152"/>
+      <c r="F28" s="152"/>
+      <c r="G28" s="152"/>
+      <c r="H28" s="152"/>
+      <c r="I28" s="152"/>
+      <c r="J28" s="152"/>
+      <c r="S28" s="162" t="s">
         <v>46</v>
       </c>
-      <c r="T28" s="162"/>
-      <c r="U28" s="152" t="s">
+      <c r="T28" s="163"/>
+      <c r="U28" s="153" t="s">
         <v>47</v>
       </c>
-      <c r="V28" s="153"/>
-      <c r="W28" s="153"/>
-      <c r="X28" s="153"/>
-      <c r="Y28" s="153"/>
-      <c r="Z28" s="153"/>
-      <c r="AA28" s="154"/>
-      <c r="AC28" s="167" t="s">
+      <c r="V28" s="154"/>
+      <c r="W28" s="154"/>
+      <c r="X28" s="154"/>
+      <c r="Y28" s="154"/>
+      <c r="Z28" s="154"/>
+      <c r="AA28" s="155"/>
+      <c r="AC28" s="168" t="s">
         <v>48</v>
       </c>
-      <c r="AD28" s="153"/>
-      <c r="AE28" s="153"/>
-      <c r="AF28" s="153"/>
-      <c r="AG28" s="153"/>
-      <c r="AH28" s="153"/>
-      <c r="AI28" s="153"/>
-      <c r="AJ28" s="154"/>
+      <c r="AD28" s="154"/>
+      <c r="AE28" s="154"/>
+      <c r="AF28" s="154"/>
+      <c r="AG28" s="154"/>
+      <c r="AH28" s="154"/>
+      <c r="AI28" s="154"/>
+      <c r="AJ28" s="155"/>
     </row>
     <row r="29" spans="1:36" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="70"/>
       <c r="B29" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="E29" s="151"/>
-      <c r="F29" s="151"/>
-      <c r="G29" s="151"/>
-      <c r="H29" s="151"/>
-      <c r="I29" s="151"/>
-      <c r="J29" s="151"/>
-      <c r="S29" s="163"/>
-      <c r="T29" s="164"/>
-      <c r="U29" s="155"/>
-      <c r="V29" s="156"/>
-      <c r="W29" s="156"/>
-      <c r="X29" s="156"/>
-      <c r="Y29" s="156"/>
-      <c r="Z29" s="156"/>
-      <c r="AA29" s="157"/>
-      <c r="AC29" s="168"/>
-      <c r="AD29" s="156"/>
-      <c r="AE29" s="156"/>
-      <c r="AF29" s="156"/>
-      <c r="AG29" s="156"/>
-      <c r="AH29" s="156"/>
-      <c r="AI29" s="156"/>
-      <c r="AJ29" s="157"/>
+      <c r="E29" s="152"/>
+      <c r="F29" s="152"/>
+      <c r="G29" s="152"/>
+      <c r="H29" s="152"/>
+      <c r="I29" s="152"/>
+      <c r="J29" s="152"/>
+      <c r="S29" s="164"/>
+      <c r="T29" s="165"/>
+      <c r="U29" s="156"/>
+      <c r="V29" s="157"/>
+      <c r="W29" s="157"/>
+      <c r="X29" s="157"/>
+      <c r="Y29" s="157"/>
+      <c r="Z29" s="157"/>
+      <c r="AA29" s="158"/>
+      <c r="AC29" s="169"/>
+      <c r="AD29" s="157"/>
+      <c r="AE29" s="157"/>
+      <c r="AF29" s="157"/>
+      <c r="AG29" s="157"/>
+      <c r="AH29" s="157"/>
+      <c r="AI29" s="157"/>
+      <c r="AJ29" s="158"/>
     </row>
     <row r="30" spans="1:36" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="71"/>
       <c r="B30" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="E30" s="151"/>
-      <c r="F30" s="151"/>
-      <c r="G30" s="151"/>
-      <c r="H30" s="151"/>
-      <c r="I30" s="151"/>
-      <c r="J30" s="151"/>
-      <c r="S30" s="163"/>
-      <c r="T30" s="164"/>
-      <c r="U30" s="155"/>
-      <c r="V30" s="156"/>
-      <c r="W30" s="156"/>
-      <c r="X30" s="156"/>
-      <c r="Y30" s="156"/>
-      <c r="Z30" s="156"/>
-      <c r="AA30" s="157"/>
-      <c r="AC30" s="168"/>
-      <c r="AD30" s="156"/>
-      <c r="AE30" s="156"/>
-      <c r="AF30" s="156"/>
-      <c r="AG30" s="156"/>
-      <c r="AH30" s="156"/>
-      <c r="AI30" s="156"/>
-      <c r="AJ30" s="157"/>
+      <c r="E30" s="152"/>
+      <c r="F30" s="152"/>
+      <c r="G30" s="152"/>
+      <c r="H30" s="152"/>
+      <c r="I30" s="152"/>
+      <c r="J30" s="152"/>
+      <c r="S30" s="164"/>
+      <c r="T30" s="165"/>
+      <c r="U30" s="156"/>
+      <c r="V30" s="157"/>
+      <c r="W30" s="157"/>
+      <c r="X30" s="157"/>
+      <c r="Y30" s="157"/>
+      <c r="Z30" s="157"/>
+      <c r="AA30" s="158"/>
+      <c r="AC30" s="169"/>
+      <c r="AD30" s="157"/>
+      <c r="AE30" s="157"/>
+      <c r="AF30" s="157"/>
+      <c r="AG30" s="157"/>
+      <c r="AH30" s="157"/>
+      <c r="AI30" s="157"/>
+      <c r="AJ30" s="158"/>
     </row>
     <row r="31" spans="1:36" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="S31" s="163"/>
-      <c r="T31" s="164"/>
-      <c r="U31" s="155"/>
-      <c r="V31" s="156"/>
-      <c r="W31" s="156"/>
-      <c r="X31" s="156"/>
-      <c r="Y31" s="156"/>
-      <c r="Z31" s="156"/>
-      <c r="AA31" s="157"/>
-      <c r="AC31" s="168"/>
-      <c r="AD31" s="156"/>
-      <c r="AE31" s="156"/>
-      <c r="AF31" s="156"/>
-      <c r="AG31" s="156"/>
-      <c r="AH31" s="156"/>
-      <c r="AI31" s="156"/>
-      <c r="AJ31" s="157"/>
+      <c r="S31" s="164"/>
+      <c r="T31" s="165"/>
+      <c r="U31" s="156"/>
+      <c r="V31" s="157"/>
+      <c r="W31" s="157"/>
+      <c r="X31" s="157"/>
+      <c r="Y31" s="157"/>
+      <c r="Z31" s="157"/>
+      <c r="AA31" s="158"/>
+      <c r="AC31" s="169"/>
+      <c r="AD31" s="157"/>
+      <c r="AE31" s="157"/>
+      <c r="AF31" s="157"/>
+      <c r="AG31" s="157"/>
+      <c r="AH31" s="157"/>
+      <c r="AI31" s="157"/>
+      <c r="AJ31" s="158"/>
     </row>
     <row r="32" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A32" s="72" t="s">
@@ -4048,29 +4122,29 @@
       <c r="F32" s="44"/>
       <c r="G32" s="44"/>
       <c r="H32" s="44"/>
-      <c r="S32" s="173"/>
-      <c r="T32" s="174"/>
-      <c r="U32" s="175"/>
-      <c r="V32" s="176"/>
-      <c r="W32" s="176"/>
-      <c r="X32" s="176"/>
-      <c r="Y32" s="176"/>
-      <c r="Z32" s="176"/>
-      <c r="AA32" s="177"/>
-      <c r="AC32" s="181"/>
-      <c r="AD32" s="176"/>
-      <c r="AE32" s="176"/>
-      <c r="AF32" s="176"/>
-      <c r="AG32" s="176"/>
-      <c r="AH32" s="176"/>
-      <c r="AI32" s="176"/>
-      <c r="AJ32" s="177"/>
+      <c r="S32" s="174"/>
+      <c r="T32" s="175"/>
+      <c r="U32" s="176"/>
+      <c r="V32" s="177"/>
+      <c r="W32" s="177"/>
+      <c r="X32" s="177"/>
+      <c r="Y32" s="177"/>
+      <c r="Z32" s="177"/>
+      <c r="AA32" s="178"/>
+      <c r="AC32" s="182"/>
+      <c r="AD32" s="177"/>
+      <c r="AE32" s="177"/>
+      <c r="AF32" s="177"/>
+      <c r="AG32" s="177"/>
+      <c r="AH32" s="177"/>
+      <c r="AI32" s="177"/>
+      <c r="AJ32" s="178"/>
     </row>
     <row r="33" spans="1:36" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="148" t="s">
+      <c r="A33" s="149" t="s">
         <v>52</v>
       </c>
-      <c r="B33" s="148"/>
+      <c r="B33" s="149"/>
       <c r="C33" s="63">
         <f>COUNTIF(D24:AG24,"=8")</f>
         <v>1</v>
@@ -4080,29 +4154,29 @@
       <c r="F33" s="44"/>
       <c r="G33" s="44"/>
       <c r="H33" s="44"/>
-      <c r="S33" s="161" t="s">
+      <c r="S33" s="162" t="s">
         <v>53</v>
       </c>
-      <c r="T33" s="162"/>
-      <c r="U33" s="152" t="s">
+      <c r="T33" s="163"/>
+      <c r="U33" s="153" t="s">
         <v>54</v>
       </c>
-      <c r="V33" s="153"/>
-      <c r="W33" s="153"/>
-      <c r="X33" s="153"/>
-      <c r="Y33" s="153"/>
-      <c r="Z33" s="153"/>
-      <c r="AA33" s="154"/>
-      <c r="AC33" s="167" t="s">
+      <c r="V33" s="154"/>
+      <c r="W33" s="154"/>
+      <c r="X33" s="154"/>
+      <c r="Y33" s="154"/>
+      <c r="Z33" s="154"/>
+      <c r="AA33" s="155"/>
+      <c r="AC33" s="168" t="s">
         <v>55</v>
       </c>
-      <c r="AD33" s="153"/>
-      <c r="AE33" s="153"/>
-      <c r="AF33" s="153"/>
-      <c r="AG33" s="153"/>
-      <c r="AH33" s="153"/>
-      <c r="AI33" s="153"/>
-      <c r="AJ33" s="154"/>
+      <c r="AD33" s="154"/>
+      <c r="AE33" s="154"/>
+      <c r="AF33" s="154"/>
+      <c r="AG33" s="154"/>
+      <c r="AH33" s="154"/>
+      <c r="AI33" s="154"/>
+      <c r="AJ33" s="155"/>
     </row>
     <row r="34" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A34" s="63" t="s">
@@ -4118,23 +4192,23 @@
       <c r="F34" s="44"/>
       <c r="G34" s="44"/>
       <c r="H34" s="44"/>
-      <c r="S34" s="163"/>
-      <c r="T34" s="164"/>
-      <c r="U34" s="155"/>
-      <c r="V34" s="156"/>
-      <c r="W34" s="156"/>
-      <c r="X34" s="156"/>
-      <c r="Y34" s="156"/>
-      <c r="Z34" s="156"/>
-      <c r="AA34" s="157"/>
-      <c r="AC34" s="168"/>
-      <c r="AD34" s="156"/>
-      <c r="AE34" s="156"/>
-      <c r="AF34" s="156"/>
-      <c r="AG34" s="156"/>
-      <c r="AH34" s="156"/>
-      <c r="AI34" s="156"/>
-      <c r="AJ34" s="157"/>
+      <c r="S34" s="164"/>
+      <c r="T34" s="165"/>
+      <c r="U34" s="156"/>
+      <c r="V34" s="157"/>
+      <c r="W34" s="157"/>
+      <c r="X34" s="157"/>
+      <c r="Y34" s="157"/>
+      <c r="Z34" s="157"/>
+      <c r="AA34" s="158"/>
+      <c r="AC34" s="169"/>
+      <c r="AD34" s="157"/>
+      <c r="AE34" s="157"/>
+      <c r="AF34" s="157"/>
+      <c r="AG34" s="157"/>
+      <c r="AH34" s="157"/>
+      <c r="AI34" s="157"/>
+      <c r="AJ34" s="158"/>
     </row>
     <row r="35" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A35" s="63" t="s">
@@ -4150,23 +4224,23 @@
       <c r="F35" s="44"/>
       <c r="G35" s="44"/>
       <c r="H35" s="44"/>
-      <c r="S35" s="163"/>
-      <c r="T35" s="164"/>
-      <c r="U35" s="155"/>
-      <c r="V35" s="156"/>
-      <c r="W35" s="156"/>
-      <c r="X35" s="156"/>
-      <c r="Y35" s="156"/>
-      <c r="Z35" s="156"/>
-      <c r="AA35" s="157"/>
-      <c r="AC35" s="168"/>
-      <c r="AD35" s="156"/>
-      <c r="AE35" s="156"/>
-      <c r="AF35" s="156"/>
-      <c r="AG35" s="156"/>
-      <c r="AH35" s="156"/>
-      <c r="AI35" s="156"/>
-      <c r="AJ35" s="157"/>
+      <c r="S35" s="164"/>
+      <c r="T35" s="165"/>
+      <c r="U35" s="156"/>
+      <c r="V35" s="157"/>
+      <c r="W35" s="157"/>
+      <c r="X35" s="157"/>
+      <c r="Y35" s="157"/>
+      <c r="Z35" s="157"/>
+      <c r="AA35" s="158"/>
+      <c r="AC35" s="169"/>
+      <c r="AD35" s="157"/>
+      <c r="AE35" s="157"/>
+      <c r="AF35" s="157"/>
+      <c r="AG35" s="157"/>
+      <c r="AH35" s="157"/>
+      <c r="AI35" s="157"/>
+      <c r="AJ35" s="158"/>
     </row>
     <row r="36" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A36" s="63" t="s">
@@ -4182,29 +4256,29 @@
       <c r="F36" s="44"/>
       <c r="G36" s="44"/>
       <c r="H36" s="44"/>
-      <c r="S36" s="163"/>
-      <c r="T36" s="164"/>
-      <c r="U36" s="155"/>
-      <c r="V36" s="156"/>
-      <c r="W36" s="156"/>
-      <c r="X36" s="156"/>
-      <c r="Y36" s="156"/>
-      <c r="Z36" s="156"/>
-      <c r="AA36" s="157"/>
-      <c r="AC36" s="168"/>
-      <c r="AD36" s="156"/>
-      <c r="AE36" s="156"/>
-      <c r="AF36" s="156"/>
-      <c r="AG36" s="156"/>
-      <c r="AH36" s="156"/>
-      <c r="AI36" s="156"/>
-      <c r="AJ36" s="157"/>
+      <c r="S36" s="164"/>
+      <c r="T36" s="165"/>
+      <c r="U36" s="156"/>
+      <c r="V36" s="157"/>
+      <c r="W36" s="157"/>
+      <c r="X36" s="157"/>
+      <c r="Y36" s="157"/>
+      <c r="Z36" s="157"/>
+      <c r="AA36" s="158"/>
+      <c r="AC36" s="169"/>
+      <c r="AD36" s="157"/>
+      <c r="AE36" s="157"/>
+      <c r="AF36" s="157"/>
+      <c r="AG36" s="157"/>
+      <c r="AH36" s="157"/>
+      <c r="AI36" s="157"/>
+      <c r="AJ36" s="158"/>
     </row>
     <row r="37" spans="1:36" ht="38.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="139" t="s">
+      <c r="A37" s="140" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="139"/>
+      <c r="B37" s="140"/>
       <c r="C37" s="63">
         <f>COUNTIF(D25:AG25,"&gt;0")</f>
         <v>20</v>
@@ -4214,23 +4288,23 @@
       <c r="F37" s="44"/>
       <c r="G37" s="44"/>
       <c r="H37" s="44"/>
-      <c r="S37" s="165"/>
-      <c r="T37" s="166"/>
-      <c r="U37" s="158"/>
-      <c r="V37" s="159"/>
-      <c r="W37" s="159"/>
-      <c r="X37" s="159"/>
-      <c r="Y37" s="159"/>
-      <c r="Z37" s="159"/>
-      <c r="AA37" s="160"/>
-      <c r="AC37" s="169"/>
-      <c r="AD37" s="159"/>
-      <c r="AE37" s="159"/>
-      <c r="AF37" s="159"/>
-      <c r="AG37" s="159"/>
-      <c r="AH37" s="159"/>
-      <c r="AI37" s="159"/>
-      <c r="AJ37" s="160"/>
+      <c r="S37" s="166"/>
+      <c r="T37" s="167"/>
+      <c r="U37" s="159"/>
+      <c r="V37" s="160"/>
+      <c r="W37" s="160"/>
+      <c r="X37" s="160"/>
+      <c r="Y37" s="160"/>
+      <c r="Z37" s="160"/>
+      <c r="AA37" s="161"/>
+      <c r="AC37" s="170"/>
+      <c r="AD37" s="160"/>
+      <c r="AE37" s="160"/>
+      <c r="AF37" s="160"/>
+      <c r="AG37" s="160"/>
+      <c r="AH37" s="160"/>
+      <c r="AI37" s="160"/>
+      <c r="AJ37" s="161"/>
     </row>
     <row r="38" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A38" s="63" t="s">
@@ -4270,10 +4344,10 @@
       <c r="H40" s="44"/>
     </row>
     <row r="41" spans="1:36" ht="35.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="139" t="s">
+      <c r="A41" s="140" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="139"/>
+      <c r="B41" s="140"/>
       <c r="C41" s="63">
         <f>AH25</f>
         <v>160</v>
@@ -4285,10 +4359,10 @@
       <c r="H41" s="44"/>
     </row>
     <row r="42" spans="1:36" ht="38.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="139" t="s">
+      <c r="A42" s="140" t="s">
         <v>63</v>
       </c>
-      <c r="B42" s="139"/>
+      <c r="B42" s="140"/>
       <c r="C42" s="63">
         <v>45</v>
       </c>
@@ -4482,10 +4556,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA136F23-B726-450C-8838-7114D5303DC9}">
-  <dimension ref="A1:AJ53"/>
+  <dimension ref="A1:AI59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4494,19 +4568,18 @@
     <col min="2" max="2" width="33.1796875" style="45" customWidth="1"/>
     <col min="3" max="3" width="10.54296875" style="42" customWidth="1"/>
     <col min="4" max="4" width="9.54296875" style="4" customWidth="1"/>
-    <col min="5" max="8" width="6.81640625" style="4" customWidth="1"/>
-    <col min="9" max="10" width="6.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="6.81640625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="7.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6328125" style="4" customWidth="1"/>
+    <col min="9" max="10" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.26953125" style="4" customWidth="1"/>
+    <col min="12" max="14" width="8" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="33" width="7.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.81640625" style="4" customWidth="1"/>
-    <col min="35" max="35" width="7.1796875" style="4" customWidth="1"/>
-    <col min="36" max="36" width="11.54296875" style="4" customWidth="1"/>
-    <col min="37" max="16384" width="8.7265625" style="4"/>
+    <col min="34" max="34" width="7.1796875" style="4" customWidth="1"/>
+    <col min="35" max="35" width="11.54296875" style="4" customWidth="1"/>
+    <col min="36" max="16384" width="8.7265625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="17" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:35" ht="17" x14ac:dyDescent="0.4">
       <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
@@ -4529,7 +4602,7 @@
       <c r="P1" s="78"/>
       <c r="Q1" s="78"/>
     </row>
-    <row r="2" spans="1:36" ht="17" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:35" ht="17" x14ac:dyDescent="0.4">
       <c r="A2" s="76" t="s">
         <v>2</v>
       </c>
@@ -4554,7 +4627,7 @@
       <c r="P2" s="78"/>
       <c r="Q2" s="78"/>
     </row>
-    <row r="3" spans="1:36" ht="17" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:35" ht="17" x14ac:dyDescent="0.4">
       <c r="A3" s="76" t="s">
         <v>4</v>
       </c>
@@ -4579,7 +4652,7 @@
       <c r="P3" s="78"/>
       <c r="Q3" s="78"/>
     </row>
-    <row r="4" spans="1:36" ht="17" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:35" ht="17" x14ac:dyDescent="0.4">
       <c r="A4" s="76"/>
       <c r="B4" s="81"/>
       <c r="C4" s="76"/>
@@ -4598,12 +4671,12 @@
       <c r="P4" s="78"/>
       <c r="Q4" s="78"/>
     </row>
-    <row r="5" spans="1:36" ht="17" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:35" ht="17" x14ac:dyDescent="0.4">
       <c r="A5" s="74" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="82" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C5" s="76"/>
       <c r="D5" s="83" t="s">
@@ -4612,7 +4685,7 @@
       <c r="E5" s="78"/>
       <c r="F5" s="78"/>
       <c r="H5" s="84" t="s">
-        <v>70</v>
+        <v>165</v>
       </c>
       <c r="I5" s="84"/>
       <c r="J5" s="78"/>
@@ -4621,19 +4694,19 @@
       </c>
       <c r="L5" s="78"/>
       <c r="M5" s="78"/>
-      <c r="N5" s="150" t="s">
-        <v>11</v>
-      </c>
-      <c r="O5" s="150"/>
-      <c r="P5" s="150"/>
-      <c r="Q5" s="150"/>
-    </row>
-    <row r="6" spans="1:36" ht="17" x14ac:dyDescent="0.4">
+      <c r="N5" s="151" t="s">
+        <v>167</v>
+      </c>
+      <c r="O5" s="151"/>
+      <c r="P5" s="151"/>
+      <c r="Q5" s="151"/>
+    </row>
+    <row r="6" spans="1:35" ht="17" x14ac:dyDescent="0.4">
       <c r="A6" s="74" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="82" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C6" s="76"/>
       <c r="D6" s="83" t="s">
@@ -4642,7 +4715,7 @@
       <c r="E6" s="78"/>
       <c r="F6" s="78"/>
       <c r="H6" s="84" t="s">
-        <v>71</v>
+        <v>166</v>
       </c>
       <c r="I6" s="84"/>
       <c r="J6" s="78"/>
@@ -4651,15 +4724,15 @@
       </c>
       <c r="L6" s="87"/>
       <c r="M6" s="76"/>
-      <c r="N6" s="149" t="s">
-        <v>17</v>
-      </c>
-      <c r="O6" s="149"/>
-      <c r="P6" s="149"/>
-      <c r="Q6" s="149"/>
+      <c r="N6" s="150" t="s">
+        <v>168</v>
+      </c>
+      <c r="O6" s="150"/>
+      <c r="P6" s="150"/>
+      <c r="Q6" s="150"/>
       <c r="W6"/>
     </row>
-    <row r="7" spans="1:36" s="42" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" s="42" customFormat="1" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="74" t="s">
         <v>18</v>
       </c>
@@ -4678,18 +4751,18 @@
       <c r="P7" s="76"/>
       <c r="Q7" s="76"/>
     </row>
-    <row r="9" spans="1:36" ht="17" x14ac:dyDescent="0.35">
-      <c r="A9" s="140" t="s">
+    <row r="9" spans="1:35" ht="17" x14ac:dyDescent="0.35">
+      <c r="A9" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="141" t="s">
+      <c r="B9" s="142" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="140" t="s">
+      <c r="C9" s="141" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="50" t="str">
-        <f t="shared" ref="D9:AH9" si="0">IFERROR(IF(D10="","",TEXT(D10,"ddd")),"")</f>
+        <f t="shared" ref="D9:AG9" si="0">IFERROR(IF(D10="","",TEXT(D10,"ddd")),"")</f>
         <v>Wed</v>
       </c>
       <c r="E9" s="50" t="str">
@@ -4808,21 +4881,17 @@
         <f t="shared" si="0"/>
         <v>Thu</v>
       </c>
-      <c r="AH9" s="50" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="AI9" s="141" t="s">
+      <c r="AH9" s="142" t="s">
         <v>23</v>
       </c>
-      <c r="AJ9" s="90" t="s">
+      <c r="AI9" s="90" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:36" ht="17" x14ac:dyDescent="0.35">
-      <c r="A10" s="140"/>
-      <c r="B10" s="141"/>
-      <c r="C10" s="140"/>
+    <row r="10" spans="1:35" ht="17" x14ac:dyDescent="0.35">
+      <c r="A10" s="141"/>
+      <c r="B10" s="142"/>
+      <c r="C10" s="141"/>
       <c r="D10" s="51" cm="1">
         <f t="array" ref="D10:AG10">IFERROR(IF(OR((B3-B2+1)&gt;31,B2="",B3=""),"",_xlfn.SEQUENCE(,B3-B2+1,B2)),"")</f>
         <v>45616</v>
@@ -4914,11 +4983,10 @@
       <c r="AG10" s="51">
         <v>45645</v>
       </c>
-      <c r="AH10" s="51"/>
-      <c r="AI10" s="141"/>
-      <c r="AJ10" s="90"/>
-    </row>
-    <row r="11" spans="1:36" ht="17" x14ac:dyDescent="0.4">
+      <c r="AH10" s="142"/>
+      <c r="AI10" s="90"/>
+    </row>
+    <row r="11" spans="1:35" ht="17" x14ac:dyDescent="0.4">
       <c r="A11" s="66" t="s">
         <v>25</v>
       </c>
@@ -4954,261 +5022,242 @@
       <c r="AE11" s="54"/>
       <c r="AF11" s="54"/>
       <c r="AG11" s="54"/>
-      <c r="AH11" s="54"/>
-      <c r="AI11" s="55"/>
-      <c r="AJ11" s="73"/>
-    </row>
-    <row r="12" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A12" s="88" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="89" t="s">
-        <v>27</v>
+      <c r="AH11" s="55"/>
+      <c r="AI11" s="73"/>
+    </row>
+    <row r="12" spans="1:35" ht="68" x14ac:dyDescent="0.4">
+      <c r="A12" s="201" t="s">
+        <v>183</v>
+      </c>
+      <c r="B12" s="139" t="s">
+        <v>172</v>
       </c>
       <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
+      <c r="D12" s="57">
+        <v>0.5</v>
+      </c>
       <c r="E12" s="57">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F12" s="57">
-        <v>0</v>
-      </c>
-      <c r="G12" s="50">
-        <v>8</v>
-      </c>
-      <c r="H12" s="57">
-        <v>5</v>
-      </c>
-      <c r="I12" s="50"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="50">
-        <v>3</v>
-      </c>
-      <c r="L12" s="50"/>
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="50"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="J12" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50">
+        <v>0.5</v>
+      </c>
       <c r="M12" s="50">
-        <v>3</v>
-      </c>
-      <c r="N12" s="50">
-        <v>2</v>
-      </c>
-      <c r="O12" s="50">
-        <v>4</v>
-      </c>
-      <c r="P12" s="50"/>
-      <c r="Q12" s="50"/>
-      <c r="R12" s="50">
-        <v>2</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="50">
+        <v>0.2</v>
+      </c>
+      <c r="Q12" s="50">
+        <v>0.2</v>
+      </c>
+      <c r="R12" s="50"/>
       <c r="S12" s="50"/>
-      <c r="T12" s="50">
-        <v>0</v>
-      </c>
-      <c r="U12" s="50">
-        <v>2</v>
-      </c>
-      <c r="V12" s="50">
-        <v>1</v>
-      </c>
-      <c r="W12" s="50">
-        <v>1</v>
-      </c>
+      <c r="T12" s="50"/>
+      <c r="U12" s="50"/>
+      <c r="V12" s="50"/>
+      <c r="W12" s="50"/>
       <c r="X12" s="50"/>
-      <c r="Y12" s="50">
-        <v>2</v>
-      </c>
-      <c r="Z12" s="50">
-        <v>4</v>
-      </c>
-      <c r="AA12" s="50">
-        <v>1</v>
-      </c>
-      <c r="AB12" s="50">
-        <v>3</v>
-      </c>
+      <c r="Y12" s="50"/>
+      <c r="Z12" s="50"/>
+      <c r="AA12" s="50"/>
+      <c r="AB12" s="50"/>
       <c r="AC12" s="50"/>
-      <c r="AD12" s="50">
-        <v>1</v>
-      </c>
+      <c r="AD12" s="50"/>
       <c r="AE12" s="50"/>
       <c r="AF12" s="57"/>
-      <c r="AG12" s="57">
-        <v>1</v>
-      </c>
-      <c r="AH12" s="57"/>
-      <c r="AI12" s="58">
-        <f>SUM(D12:AH12)</f>
-        <v>43</v>
-      </c>
-      <c r="AJ12" s="73"/>
-    </row>
-    <row r="13" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="B13" s="89" t="s">
-        <v>28</v>
+      <c r="AG12" s="57"/>
+      <c r="AH12" s="58">
+        <f>SUM(D12:AG12)</f>
+        <v>3.9000000000000004</v>
+      </c>
+      <c r="AI12" s="73"/>
+    </row>
+    <row r="13" spans="1:35" ht="68" x14ac:dyDescent="0.4">
+      <c r="A13" s="202"/>
+      <c r="B13" s="139" t="s">
+        <v>173</v>
       </c>
       <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="57"/>
+      <c r="D13" s="57">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="57">
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="57">
+        <v>0.5</v>
+      </c>
       <c r="G13" s="50"/>
       <c r="H13" s="57"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="50">
-        <v>1</v>
-      </c>
-      <c r="L13" s="50"/>
+      <c r="I13" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="J13" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50">
+        <v>0.5</v>
+      </c>
       <c r="M13" s="50">
-        <v>1</v>
-      </c>
-      <c r="N13" s="50">
-        <v>4</v>
-      </c>
-      <c r="O13" s="50">
-        <v>3</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="N13" s="50"/>
+      <c r="O13" s="50"/>
       <c r="P13" s="50"/>
       <c r="Q13" s="50"/>
       <c r="R13" s="50">
-        <v>4</v>
-      </c>
-      <c r="S13" s="50"/>
-      <c r="T13" s="50"/>
-      <c r="U13" s="50">
-        <v>4</v>
-      </c>
-      <c r="V13" s="50">
-        <v>4</v>
-      </c>
-      <c r="W13" s="50">
-        <v>4</v>
-      </c>
+        <v>0.2</v>
+      </c>
+      <c r="S13" s="50">
+        <v>0.2</v>
+      </c>
+      <c r="T13" s="50">
+        <v>0.2</v>
+      </c>
+      <c r="U13" s="50"/>
+      <c r="V13" s="50"/>
+      <c r="W13" s="50"/>
       <c r="X13" s="50"/>
-      <c r="Y13" s="50">
-        <v>3</v>
-      </c>
-      <c r="Z13" s="50">
-        <v>2</v>
-      </c>
-      <c r="AA13" s="50">
-        <v>2</v>
-      </c>
-      <c r="AB13" s="50">
-        <v>3</v>
-      </c>
-      <c r="AC13" s="50">
-        <v>5</v>
-      </c>
-      <c r="AD13" s="50">
-        <v>2</v>
-      </c>
+      <c r="Y13" s="50"/>
+      <c r="Z13" s="50"/>
+      <c r="AA13" s="50"/>
+      <c r="AB13" s="50"/>
+      <c r="AC13" s="50"/>
+      <c r="AD13" s="50"/>
       <c r="AE13" s="50"/>
       <c r="AF13" s="57"/>
-      <c r="AG13" s="57">
-        <v>3</v>
-      </c>
-      <c r="AH13" s="57"/>
-      <c r="AI13" s="58">
-        <f>SUM(D13:AH13)</f>
-        <v>45</v>
-      </c>
-      <c r="AJ13" s="73"/>
-    </row>
-    <row r="14" spans="1:36" ht="34" x14ac:dyDescent="0.4">
-      <c r="A14" s="89" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="89" t="s">
-        <v>30</v>
+      <c r="AG13" s="57"/>
+      <c r="AH13" s="58">
+        <f>SUM(D13:AG13)</f>
+        <v>4.1000000000000005</v>
+      </c>
+      <c r="AI13" s="73"/>
+    </row>
+    <row r="14" spans="1:35" ht="68" x14ac:dyDescent="0.4">
+      <c r="A14" s="202"/>
+      <c r="B14" s="139" t="s">
+        <v>174</v>
       </c>
       <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
+      <c r="D14" s="57">
+        <v>0.5</v>
+      </c>
+      <c r="E14" s="57">
+        <v>0.5</v>
+      </c>
+      <c r="F14" s="57">
+        <v>0.5</v>
+      </c>
       <c r="G14" s="50"/>
       <c r="H14" s="57"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="50">
-        <v>2</v>
-      </c>
-      <c r="L14" s="50"/>
+      <c r="I14" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="J14" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="K14" s="50"/>
+      <c r="L14" s="50">
+        <v>0.5</v>
+      </c>
       <c r="M14" s="50">
-        <v>1</v>
-      </c>
-      <c r="N14" s="50">
-        <v>1</v>
-      </c>
-      <c r="O14" s="50">
-        <v>1</v>
-      </c>
-      <c r="P14" s="50">
-        <v>6</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="N14" s="50"/>
+      <c r="O14" s="50"/>
+      <c r="P14" s="50"/>
       <c r="Q14" s="50"/>
       <c r="R14" s="50">
-        <v>1</v>
-      </c>
-      <c r="S14" s="50"/>
-      <c r="T14" s="50"/>
-      <c r="U14" s="50">
-        <v>1</v>
-      </c>
-      <c r="V14" s="50">
-        <v>1</v>
-      </c>
-      <c r="W14" s="50">
-        <v>1</v>
-      </c>
+        <v>0.2</v>
+      </c>
+      <c r="S14" s="50">
+        <v>0.2</v>
+      </c>
+      <c r="T14" s="50">
+        <v>0.2</v>
+      </c>
+      <c r="U14" s="50"/>
+      <c r="V14" s="50"/>
+      <c r="W14" s="50"/>
       <c r="X14" s="50"/>
-      <c r="Y14" s="50">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="50">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="50">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="50">
-        <v>5</v>
-      </c>
+      <c r="Y14" s="50"/>
+      <c r="Z14" s="50"/>
+      <c r="AA14" s="50"/>
+      <c r="AB14" s="50"/>
       <c r="AC14" s="50"/>
-      <c r="AD14" s="50">
-        <v>0</v>
-      </c>
+      <c r="AD14" s="50"/>
       <c r="AE14" s="50"/>
       <c r="AF14" s="57"/>
-      <c r="AG14" s="57">
-        <v>2</v>
-      </c>
-      <c r="AH14" s="57"/>
-      <c r="AI14" s="58">
-        <f>SUM(D14:AH14)</f>
-        <v>22</v>
-      </c>
-      <c r="AJ14" s="73"/>
-    </row>
-    <row r="15" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A15" s="67"/>
-      <c r="B15" s="56"/>
+      <c r="AG14" s="57"/>
+      <c r="AH14" s="58">
+        <f>SUM(D14:AG14)</f>
+        <v>4.1000000000000005</v>
+      </c>
+      <c r="AI14" s="73"/>
+    </row>
+    <row r="15" spans="1:35" ht="68" x14ac:dyDescent="0.4">
+      <c r="A15" s="202"/>
+      <c r="B15" s="139" t="s">
+        <v>175</v>
+      </c>
       <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
+      <c r="D15" s="57">
+        <v>1.5</v>
+      </c>
+      <c r="E15" s="57">
+        <v>1.5</v>
+      </c>
+      <c r="F15" s="57">
+        <v>1.5</v>
+      </c>
       <c r="G15" s="50"/>
       <c r="H15" s="57"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="50"/>
+      <c r="I15" s="50">
+        <v>1.5</v>
+      </c>
+      <c r="J15" s="50">
+        <v>1.5</v>
+      </c>
       <c r="K15" s="50"/>
-      <c r="L15" s="50"/>
-      <c r="M15" s="50"/>
+      <c r="L15" s="50">
+        <v>1.5</v>
+      </c>
+      <c r="M15" s="50">
+        <v>1.5</v>
+      </c>
       <c r="N15" s="50"/>
       <c r="O15" s="50"/>
-      <c r="P15" s="50"/>
-      <c r="Q15" s="50"/>
-      <c r="R15" s="50"/>
-      <c r="S15" s="50"/>
-      <c r="T15" s="50"/>
+      <c r="P15" s="50">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="50">
+        <v>1</v>
+      </c>
+      <c r="R15" s="50">
+        <v>1</v>
+      </c>
+      <c r="S15" s="50">
+        <v>1</v>
+      </c>
+      <c r="T15" s="50">
+        <v>1</v>
+      </c>
       <c r="U15" s="50"/>
       <c r="V15" s="50"/>
       <c r="W15" s="50"/>
@@ -5222,24 +5271,42 @@
       <c r="AE15" s="50"/>
       <c r="AF15" s="57"/>
       <c r="AG15" s="57"/>
-      <c r="AH15" s="57"/>
-      <c r="AI15" s="58"/>
-      <c r="AJ15" s="73"/>
-    </row>
-    <row r="16" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A16" s="67"/>
-      <c r="B16" s="56"/>
+      <c r="AH15" s="58">
+        <f t="shared" ref="AH15:AH17" si="1">SUM(D15:AG15)</f>
+        <v>15.5</v>
+      </c>
+      <c r="AI15" s="73"/>
+    </row>
+    <row r="16" spans="1:35" ht="85" x14ac:dyDescent="0.4">
+      <c r="A16" s="202"/>
+      <c r="B16" s="139" t="s">
+        <v>176</v>
+      </c>
       <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
+      <c r="D16" s="57">
+        <v>1.5</v>
+      </c>
+      <c r="E16" s="57">
+        <v>1.5</v>
+      </c>
+      <c r="F16" s="57">
+        <v>1.5</v>
+      </c>
       <c r="G16" s="50"/>
       <c r="H16" s="57"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="50"/>
+      <c r="I16" s="50">
+        <v>1.5</v>
+      </c>
+      <c r="J16" s="50">
+        <v>1.5</v>
+      </c>
       <c r="K16" s="50"/>
-      <c r="L16" s="50"/>
-      <c r="M16" s="50"/>
+      <c r="L16" s="50">
+        <v>1.5</v>
+      </c>
+      <c r="M16" s="50">
+        <v>1.5</v>
+      </c>
       <c r="N16" s="50"/>
       <c r="O16" s="50"/>
       <c r="P16" s="50"/>
@@ -5260,149 +5327,135 @@
       <c r="AE16" s="50"/>
       <c r="AF16" s="57"/>
       <c r="AG16" s="57"/>
-      <c r="AH16" s="57"/>
-      <c r="AI16" s="58"/>
-      <c r="AJ16" s="73"/>
-    </row>
-    <row r="17" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A17" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="59"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="54"/>
-      <c r="L17" s="54"/>
-      <c r="M17" s="54"/>
-      <c r="N17" s="54"/>
-      <c r="O17" s="54"/>
-      <c r="P17" s="54"/>
-      <c r="Q17" s="54"/>
-      <c r="R17" s="54"/>
-      <c r="S17" s="54"/>
-      <c r="T17" s="54"/>
-      <c r="U17" s="54"/>
-      <c r="V17" s="54"/>
-      <c r="W17" s="54"/>
-      <c r="X17" s="54"/>
-      <c r="Y17" s="54"/>
-      <c r="Z17" s="54"/>
-      <c r="AA17" s="54"/>
-      <c r="AB17" s="54"/>
-      <c r="AC17" s="54"/>
-      <c r="AD17" s="54"/>
-      <c r="AE17" s="54"/>
-      <c r="AF17" s="54"/>
-      <c r="AG17" s="54"/>
-      <c r="AH17" s="54"/>
-      <c r="AI17" s="55"/>
-      <c r="AJ17" s="73"/>
-    </row>
-    <row r="18" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A18" s="67"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="57" t="s">
-        <v>34</v>
-      </c>
+      <c r="AH16" s="58">
+        <f t="shared" si="1"/>
+        <v>10.5</v>
+      </c>
+      <c r="AI16" s="73"/>
+    </row>
+    <row r="17" spans="1:35" ht="102" x14ac:dyDescent="0.4">
+      <c r="A17" s="202"/>
+      <c r="B17" s="139" t="s">
+        <v>177</v>
+      </c>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57">
+        <v>1.5</v>
+      </c>
+      <c r="E17" s="57">
+        <v>1.5</v>
+      </c>
+      <c r="F17" s="57">
+        <v>1.5</v>
+      </c>
+      <c r="G17" s="50"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="50">
+        <v>1.5</v>
+      </c>
+      <c r="J17" s="50">
+        <v>1.5</v>
+      </c>
+      <c r="K17" s="50"/>
+      <c r="L17" s="50">
+        <v>1.5</v>
+      </c>
+      <c r="M17" s="50">
+        <v>1.5</v>
+      </c>
+      <c r="N17" s="50"/>
+      <c r="O17" s="50"/>
+      <c r="P17" s="50"/>
+      <c r="Q17" s="50"/>
+      <c r="R17" s="50"/>
+      <c r="S17" s="50"/>
+      <c r="T17" s="50"/>
+      <c r="U17" s="50"/>
+      <c r="V17" s="50"/>
+      <c r="W17" s="50"/>
+      <c r="X17" s="50"/>
+      <c r="Y17" s="50"/>
+      <c r="Z17" s="50"/>
+      <c r="AA17" s="50"/>
+      <c r="AB17" s="50"/>
+      <c r="AC17" s="50"/>
+      <c r="AD17" s="50"/>
+      <c r="AE17" s="50"/>
+      <c r="AF17" s="57"/>
+      <c r="AG17" s="57"/>
+      <c r="AH17" s="58">
+        <f t="shared" si="1"/>
+        <v>10.5</v>
+      </c>
+      <c r="AI17" s="73"/>
+    </row>
+    <row r="18" spans="1:35" ht="136" x14ac:dyDescent="0.4">
+      <c r="A18" s="202"/>
+      <c r="B18" s="139" t="s">
+        <v>178</v>
+      </c>
+      <c r="C18" s="57"/>
       <c r="D18" s="57"/>
       <c r="E18" s="57">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F18" s="57">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G18" s="50"/>
-      <c r="H18" s="57">
-        <v>3</v>
-      </c>
+      <c r="H18" s="57"/>
       <c r="I18" s="50"/>
       <c r="J18" s="50"/>
-      <c r="K18" s="50">
-        <v>1</v>
-      </c>
+      <c r="K18" s="50"/>
       <c r="L18" s="50"/>
-      <c r="M18" s="50">
-        <v>2</v>
-      </c>
+      <c r="M18" s="50"/>
       <c r="N18" s="50"/>
       <c r="O18" s="50"/>
       <c r="P18" s="50"/>
       <c r="Q18" s="50"/>
-      <c r="R18" s="50">
-        <v>1</v>
-      </c>
+      <c r="R18" s="50"/>
       <c r="S18" s="50"/>
       <c r="T18" s="50"/>
-      <c r="U18" s="50">
-        <v>1</v>
-      </c>
-      <c r="V18" s="50">
-        <v>2</v>
-      </c>
-      <c r="W18" s="50">
-        <v>2</v>
-      </c>
+      <c r="U18" s="50"/>
+      <c r="V18" s="50"/>
+      <c r="W18" s="50"/>
       <c r="X18" s="50"/>
-      <c r="Y18" s="50">
-        <v>1</v>
-      </c>
-      <c r="Z18" s="50">
-        <v>2</v>
-      </c>
-      <c r="AA18" s="50">
-        <v>4</v>
-      </c>
-      <c r="AB18" s="50">
-        <v>2</v>
-      </c>
+      <c r="Y18" s="50"/>
+      <c r="Z18" s="50"/>
+      <c r="AA18" s="50"/>
+      <c r="AB18" s="50"/>
       <c r="AC18" s="50"/>
-      <c r="AD18" s="50">
-        <v>4</v>
-      </c>
+      <c r="AD18" s="50"/>
       <c r="AE18" s="50"/>
       <c r="AF18" s="57"/>
       <c r="AG18" s="57"/>
-      <c r="AH18" s="57"/>
-      <c r="AI18" s="58">
-        <f>SUM(D18:AH18)</f>
-        <v>25</v>
-      </c>
-      <c r="AJ18" s="73"/>
-    </row>
-    <row r="19" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A19" s="67"/>
-      <c r="B19" s="56"/>
-      <c r="C19" s="57" t="s">
-        <v>36</v>
-      </c>
+      <c r="AH18" s="58"/>
+      <c r="AI18" s="73"/>
+    </row>
+    <row r="19" spans="1:35" ht="136" x14ac:dyDescent="0.4">
+      <c r="A19" s="202"/>
+      <c r="B19" s="139" t="s">
+        <v>179</v>
+      </c>
+      <c r="C19" s="57"/>
       <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
+      <c r="E19" s="57">
+        <v>0.5</v>
+      </c>
+      <c r="F19" s="57">
+        <v>0.5</v>
+      </c>
       <c r="G19" s="50"/>
       <c r="H19" s="57"/>
-      <c r="I19" s="50">
-        <v>2</v>
-      </c>
+      <c r="I19" s="50"/>
       <c r="J19" s="50"/>
-      <c r="K19" s="50">
-        <v>1</v>
-      </c>
+      <c r="K19" s="50"/>
       <c r="L19" s="50"/>
       <c r="M19" s="50"/>
       <c r="N19" s="50"/>
       <c r="O19" s="50"/>
-      <c r="P19" s="50">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="50">
-        <v>1</v>
-      </c>
+      <c r="P19" s="50"/>
+      <c r="Q19" s="50"/>
       <c r="R19" s="50"/>
       <c r="S19" s="50"/>
       <c r="T19" s="50"/>
@@ -5410,12 +5463,8 @@
       <c r="V19" s="50"/>
       <c r="W19" s="50"/>
       <c r="X19" s="50"/>
-      <c r="Y19" s="50">
-        <v>1</v>
-      </c>
-      <c r="Z19" s="50">
-        <v>1</v>
-      </c>
+      <c r="Y19" s="50"/>
+      <c r="Z19" s="50"/>
       <c r="AA19" s="50"/>
       <c r="AB19" s="50"/>
       <c r="AC19" s="50"/>
@@ -5423,45 +5472,29 @@
       <c r="AE19" s="50"/>
       <c r="AF19" s="57"/>
       <c r="AG19" s="57"/>
-      <c r="AH19" s="57"/>
-      <c r="AI19" s="58">
-        <f>SUM(D19:AH19)</f>
-        <v>7</v>
-      </c>
-      <c r="AJ19" s="73"/>
-    </row>
-    <row r="20" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A20" s="67"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="57" t="s">
-        <v>37</v>
-      </c>
+      <c r="AH19" s="58"/>
+      <c r="AI19" s="73"/>
+    </row>
+    <row r="20" spans="1:35" ht="136" x14ac:dyDescent="0.4">
+      <c r="A20" s="202"/>
+      <c r="B20" s="139" t="s">
+        <v>180</v>
+      </c>
+      <c r="C20" s="57"/>
       <c r="D20" s="57"/>
       <c r="E20" s="57"/>
       <c r="F20" s="57"/>
       <c r="G20" s="50"/>
       <c r="H20" s="57"/>
-      <c r="I20" s="50">
-        <v>2</v>
-      </c>
+      <c r="I20" s="50"/>
       <c r="J20" s="50"/>
-      <c r="K20" s="50">
-        <v>2</v>
-      </c>
+      <c r="K20" s="50"/>
       <c r="L20" s="50"/>
-      <c r="M20" s="50">
-        <v>1</v>
-      </c>
-      <c r="N20" s="50">
-        <v>3</v>
-      </c>
+      <c r="M20" s="50"/>
+      <c r="N20" s="50"/>
       <c r="O20" s="50"/>
-      <c r="P20" s="50">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="50">
-        <v>1</v>
-      </c>
+      <c r="P20" s="50"/>
+      <c r="Q20" s="50"/>
       <c r="R20" s="50"/>
       <c r="S20" s="50"/>
       <c r="T20" s="50"/>
@@ -5469,76 +5502,63 @@
       <c r="V20" s="50"/>
       <c r="W20" s="50"/>
       <c r="X20" s="50"/>
-      <c r="Y20" s="50">
-        <v>3</v>
-      </c>
-      <c r="Z20" s="50">
-        <v>1</v>
-      </c>
-      <c r="AA20" s="50">
-        <v>1</v>
-      </c>
+      <c r="Y20" s="50"/>
+      <c r="Z20" s="50"/>
+      <c r="AA20" s="50"/>
       <c r="AB20" s="50"/>
       <c r="AC20" s="50"/>
-      <c r="AD20" s="50">
-        <v>1</v>
-      </c>
+      <c r="AD20" s="50"/>
       <c r="AE20" s="50"/>
       <c r="AF20" s="57"/>
-      <c r="AG20" s="57">
-        <v>2</v>
-      </c>
-      <c r="AH20" s="57"/>
-      <c r="AI20" s="58">
-        <f>SUM(D20:AH20)</f>
-        <v>18</v>
-      </c>
-      <c r="AJ20" s="73"/>
-    </row>
-    <row r="21" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="68"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="61"/>
-      <c r="D21" s="61"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="61"/>
-      <c r="H21" s="61"/>
-      <c r="I21" s="61"/>
-      <c r="J21" s="61"/>
-      <c r="K21" s="61"/>
-      <c r="L21" s="61"/>
-      <c r="M21" s="61"/>
-      <c r="N21" s="61"/>
-      <c r="O21" s="61"/>
-      <c r="P21" s="61"/>
-      <c r="Q21" s="61"/>
-      <c r="R21" s="61"/>
-      <c r="S21" s="61"/>
-      <c r="T21" s="61"/>
-      <c r="U21" s="61"/>
-      <c r="V21" s="61"/>
-      <c r="W21" s="61"/>
-      <c r="X21" s="61"/>
-      <c r="Y21" s="61"/>
-      <c r="Z21" s="61"/>
-      <c r="AA21" s="61"/>
-      <c r="AB21" s="61"/>
-      <c r="AC21" s="61"/>
-      <c r="AD21" s="61"/>
-      <c r="AE21" s="61"/>
-      <c r="AF21" s="61"/>
-      <c r="AG21" s="62"/>
-      <c r="AH21" s="62"/>
-      <c r="AI21" s="62"/>
-      <c r="AJ21" s="73"/>
-    </row>
-    <row r="22" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A22" s="142" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="143"/>
-      <c r="C22" s="144"/>
+      <c r="AG20" s="57"/>
+      <c r="AH20" s="58"/>
+      <c r="AI20" s="73"/>
+    </row>
+    <row r="21" spans="1:35" ht="228" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="203"/>
+      <c r="B21" s="139" t="s">
+        <v>181</v>
+      </c>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57">
+        <v>1</v>
+      </c>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="50"/>
+      <c r="N21" s="50"/>
+      <c r="O21" s="50"/>
+      <c r="P21" s="50"/>
+      <c r="Q21" s="50"/>
+      <c r="R21" s="50"/>
+      <c r="S21" s="50"/>
+      <c r="T21" s="50"/>
+      <c r="U21" s="50"/>
+      <c r="V21" s="50"/>
+      <c r="W21" s="50"/>
+      <c r="X21" s="50"/>
+      <c r="Y21" s="50"/>
+      <c r="Z21" s="50"/>
+      <c r="AA21" s="50"/>
+      <c r="AB21" s="50"/>
+      <c r="AC21" s="50"/>
+      <c r="AD21" s="50"/>
+      <c r="AE21" s="50"/>
+      <c r="AF21" s="57"/>
+      <c r="AG21" s="57"/>
+      <c r="AH21" s="58"/>
+      <c r="AI21" s="73"/>
+    </row>
+    <row r="22" spans="1:35" ht="17" x14ac:dyDescent="0.4">
+      <c r="A22" s="89"/>
+      <c r="B22" s="89"/>
+      <c r="C22" s="57"/>
       <c r="D22" s="57"/>
       <c r="E22" s="57"/>
       <c r="F22" s="57"/>
@@ -5569,79 +5589,95 @@
       <c r="AE22" s="50"/>
       <c r="AF22" s="57"/>
       <c r="AG22" s="57"/>
-      <c r="AH22" s="57"/>
-      <c r="AI22" s="58">
-        <f>SUM(D22:AH22)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ22" s="73"/>
-    </row>
-    <row r="23" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A23" s="142" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="143"/>
-      <c r="C23" s="144"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="50"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="50"/>
-      <c r="O23" s="50"/>
-      <c r="P23" s="50"/>
-      <c r="Q23" s="50"/>
-      <c r="R23" s="50"/>
-      <c r="S23" s="50"/>
-      <c r="T23" s="50"/>
-      <c r="U23" s="50"/>
-      <c r="V23" s="50"/>
-      <c r="W23" s="50"/>
-      <c r="X23" s="50"/>
-      <c r="Y23" s="50"/>
-      <c r="Z23" s="50"/>
-      <c r="AA23" s="50"/>
-      <c r="AB23" s="50"/>
-      <c r="AC23" s="50"/>
-      <c r="AD23" s="50"/>
-      <c r="AE23" s="50"/>
-      <c r="AF23" s="57"/>
-      <c r="AG23" s="57"/>
-      <c r="AH23" s="57"/>
-      <c r="AI23" s="58">
-        <f>SUM(D23:AH23)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ23" s="73"/>
-    </row>
-    <row r="24" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A24" s="145" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="146"/>
-      <c r="C24" s="147"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="57"/>
+      <c r="AH22" s="58"/>
+      <c r="AI22" s="73"/>
+    </row>
+    <row r="23" spans="1:35" ht="17" x14ac:dyDescent="0.4">
+      <c r="A23" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="59"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="54"/>
+      <c r="N23" s="54"/>
+      <c r="O23" s="54"/>
+      <c r="P23" s="54"/>
+      <c r="Q23" s="54"/>
+      <c r="R23" s="54"/>
+      <c r="S23" s="54"/>
+      <c r="T23" s="54"/>
+      <c r="U23" s="54"/>
+      <c r="V23" s="54"/>
+      <c r="W23" s="54"/>
+      <c r="X23" s="54"/>
+      <c r="Y23" s="54"/>
+      <c r="Z23" s="54"/>
+      <c r="AA23" s="54"/>
+      <c r="AB23" s="54"/>
+      <c r="AC23" s="54"/>
+      <c r="AD23" s="54"/>
+      <c r="AE23" s="54"/>
+      <c r="AF23" s="54"/>
+      <c r="AG23" s="54"/>
+      <c r="AH23" s="55"/>
+      <c r="AI23" s="73"/>
+    </row>
+    <row r="24" spans="1:35" ht="17" x14ac:dyDescent="0.4">
+      <c r="A24" s="67"/>
+      <c r="B24" s="56" t="s">
+        <v>169</v>
+      </c>
+      <c r="C24" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="57">
+        <v>1</v>
+      </c>
+      <c r="E24" s="57">
+        <v>1</v>
+      </c>
+      <c r="F24" s="57">
+        <v>1</v>
+      </c>
       <c r="G24" s="50"/>
       <c r="H24" s="57"/>
-      <c r="I24" s="50"/>
-      <c r="J24" s="50"/>
+      <c r="I24" s="50">
+        <v>1</v>
+      </c>
+      <c r="J24" s="50">
+        <v>1</v>
+      </c>
       <c r="K24" s="50"/>
-      <c r="L24" s="50"/>
-      <c r="M24" s="50"/>
+      <c r="L24" s="50">
+        <v>1</v>
+      </c>
+      <c r="M24" s="50">
+        <v>1</v>
+      </c>
       <c r="N24" s="50"/>
       <c r="O24" s="50"/>
       <c r="P24" s="50"/>
-      <c r="Q24" s="50"/>
-      <c r="R24" s="50"/>
-      <c r="S24" s="50"/>
-      <c r="T24" s="50"/>
+      <c r="Q24" s="50">
+        <v>1</v>
+      </c>
+      <c r="R24" s="50">
+        <v>1</v>
+      </c>
+      <c r="S24" s="50">
+        <v>1</v>
+      </c>
+      <c r="T24" s="50">
+        <v>1</v>
+      </c>
       <c r="U24" s="50"/>
       <c r="V24" s="50"/>
       <c r="W24" s="50"/>
@@ -5655,663 +5691,840 @@
       <c r="AE24" s="50"/>
       <c r="AF24" s="57"/>
       <c r="AG24" s="57"/>
-      <c r="AH24" s="57"/>
-      <c r="AI24" s="58">
-        <f>SUM(D24:AH24)</f>
+      <c r="AH24" s="58">
+        <f>SUM(D24:AG24)</f>
+        <v>11</v>
+      </c>
+      <c r="AI24" s="73"/>
+    </row>
+    <row r="25" spans="1:35" ht="17" x14ac:dyDescent="0.4">
+      <c r="A25" s="67"/>
+      <c r="B25" s="56" t="s">
+        <v>182</v>
+      </c>
+      <c r="C25" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="50"/>
+      <c r="L25" s="50"/>
+      <c r="M25" s="50"/>
+      <c r="N25" s="50"/>
+      <c r="O25" s="50"/>
+      <c r="P25" s="50"/>
+      <c r="Q25" s="50"/>
+      <c r="R25" s="50"/>
+      <c r="S25" s="50">
+        <v>2</v>
+      </c>
+      <c r="T25" s="50">
+        <v>1</v>
+      </c>
+      <c r="U25" s="50"/>
+      <c r="V25" s="50"/>
+      <c r="W25" s="50"/>
+      <c r="X25" s="50"/>
+      <c r="Y25" s="50"/>
+      <c r="Z25" s="50"/>
+      <c r="AA25" s="50"/>
+      <c r="AB25" s="50"/>
+      <c r="AC25" s="50"/>
+      <c r="AD25" s="50"/>
+      <c r="AE25" s="50"/>
+      <c r="AF25" s="57"/>
+      <c r="AG25" s="57"/>
+      <c r="AH25" s="58">
+        <f>SUM(D25:AG25)</f>
+        <v>3</v>
+      </c>
+      <c r="AI25" s="73"/>
+    </row>
+    <row r="26" spans="1:35" ht="17" x14ac:dyDescent="0.4">
+      <c r="A26" s="67"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="50"/>
+      <c r="L26" s="50"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="50"/>
+      <c r="O26" s="50"/>
+      <c r="P26" s="50"/>
+      <c r="Q26" s="50"/>
+      <c r="R26" s="50"/>
+      <c r="S26" s="50"/>
+      <c r="T26" s="50"/>
+      <c r="U26" s="50"/>
+      <c r="V26" s="50"/>
+      <c r="W26" s="50"/>
+      <c r="X26" s="50"/>
+      <c r="Y26" s="50"/>
+      <c r="Z26" s="50"/>
+      <c r="AA26" s="50"/>
+      <c r="AB26" s="50"/>
+      <c r="AC26" s="50"/>
+      <c r="AD26" s="50"/>
+      <c r="AE26" s="50"/>
+      <c r="AF26" s="57"/>
+      <c r="AG26" s="57"/>
+      <c r="AH26" s="58">
+        <f>SUM(D26:AG26)</f>
         <v>0</v>
       </c>
-      <c r="AJ24" s="73"/>
-    </row>
-    <row r="25" spans="1:36" ht="17" x14ac:dyDescent="0.4">
-      <c r="A25" s="142" t="s">
+      <c r="AI26" s="73"/>
+    </row>
+    <row r="27" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="68"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="61"/>
+      <c r="J27" s="61"/>
+      <c r="K27" s="61"/>
+      <c r="L27" s="61"/>
+      <c r="M27" s="61"/>
+      <c r="N27" s="61"/>
+      <c r="O27" s="61"/>
+      <c r="P27" s="61"/>
+      <c r="Q27" s="61"/>
+      <c r="R27" s="61"/>
+      <c r="S27" s="61"/>
+      <c r="T27" s="61"/>
+      <c r="U27" s="61"/>
+      <c r="V27" s="61"/>
+      <c r="W27" s="61"/>
+      <c r="X27" s="61"/>
+      <c r="Y27" s="61"/>
+      <c r="Z27" s="61"/>
+      <c r="AA27" s="61"/>
+      <c r="AB27" s="61"/>
+      <c r="AC27" s="61"/>
+      <c r="AD27" s="61"/>
+      <c r="AE27" s="61"/>
+      <c r="AF27" s="61"/>
+      <c r="AG27" s="62"/>
+      <c r="AH27" s="62"/>
+      <c r="AI27" s="73"/>
+    </row>
+    <row r="28" spans="1:35" ht="17" x14ac:dyDescent="0.4">
+      <c r="A28" s="143" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="144"/>
+      <c r="C28" s="145"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="50"/>
+      <c r="N28" s="50"/>
+      <c r="O28" s="50"/>
+      <c r="P28" s="50"/>
+      <c r="Q28" s="50"/>
+      <c r="R28" s="50"/>
+      <c r="S28" s="50"/>
+      <c r="T28" s="50"/>
+      <c r="U28" s="50"/>
+      <c r="V28" s="50"/>
+      <c r="W28" s="50">
+        <v>8</v>
+      </c>
+      <c r="X28" s="50">
+        <v>8</v>
+      </c>
+      <c r="Y28" s="50">
+        <v>8</v>
+      </c>
+      <c r="Z28" s="50">
+        <v>8</v>
+      </c>
+      <c r="AA28" s="50">
+        <v>8</v>
+      </c>
+      <c r="AB28" s="50"/>
+      <c r="AC28" s="50"/>
+      <c r="AD28" s="50">
+        <v>8</v>
+      </c>
+      <c r="AE28" s="50">
+        <v>8</v>
+      </c>
+      <c r="AF28" s="57">
+        <v>8</v>
+      </c>
+      <c r="AG28" s="57">
+        <v>8</v>
+      </c>
+      <c r="AH28" s="58">
+        <f>SUM(D28:AG28)</f>
+        <v>72</v>
+      </c>
+      <c r="AI28" s="73"/>
+    </row>
+    <row r="29" spans="1:35" ht="17" x14ac:dyDescent="0.4">
+      <c r="A29" s="143" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="144"/>
+      <c r="C29" s="145"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="50"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="50"/>
+      <c r="N29" s="50"/>
+      <c r="O29" s="50"/>
+      <c r="P29" s="50">
+        <v>8</v>
+      </c>
+      <c r="Q29" s="50"/>
+      <c r="R29" s="50"/>
+      <c r="S29" s="50"/>
+      <c r="T29" s="50"/>
+      <c r="U29" s="50"/>
+      <c r="V29" s="50"/>
+      <c r="W29" s="50"/>
+      <c r="X29" s="50"/>
+      <c r="Y29" s="50"/>
+      <c r="Z29" s="50"/>
+      <c r="AA29" s="50"/>
+      <c r="AB29" s="50"/>
+      <c r="AC29" s="50"/>
+      <c r="AD29" s="50"/>
+      <c r="AE29" s="50"/>
+      <c r="AF29" s="57"/>
+      <c r="AG29" s="57"/>
+      <c r="AH29" s="58">
+        <f>SUM(D29:AG29)</f>
+        <v>8</v>
+      </c>
+      <c r="AI29" s="73"/>
+    </row>
+    <row r="30" spans="1:35" ht="17" x14ac:dyDescent="0.4">
+      <c r="A30" s="146" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="147"/>
+      <c r="C30" s="148"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="50"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="50">
+        <v>8</v>
+      </c>
+      <c r="L30" s="50"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="50"/>
+      <c r="O30" s="50"/>
+      <c r="P30" s="50"/>
+      <c r="Q30" s="50"/>
+      <c r="R30" s="50"/>
+      <c r="S30" s="50"/>
+      <c r="T30" s="50"/>
+      <c r="U30" s="50"/>
+      <c r="V30" s="50"/>
+      <c r="W30" s="50"/>
+      <c r="X30" s="50"/>
+      <c r="Y30" s="50"/>
+      <c r="Z30" s="50"/>
+      <c r="AA30" s="50"/>
+      <c r="AB30" s="50"/>
+      <c r="AC30" s="50"/>
+      <c r="AD30" s="50"/>
+      <c r="AE30" s="50"/>
+      <c r="AF30" s="57"/>
+      <c r="AG30" s="57"/>
+      <c r="AH30" s="58">
+        <f>SUM(D30:AG30)</f>
+        <v>8</v>
+      </c>
+      <c r="AI30" s="73"/>
+    </row>
+    <row r="31" spans="1:35" ht="17" x14ac:dyDescent="0.4">
+      <c r="A31" s="143" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="143"/>
-      <c r="C25" s="144"/>
-      <c r="D25" s="57">
-        <f t="shared" ref="D25:AB25" si="1">SUM(D11:D20)</f>
+      <c r="B31" s="144"/>
+      <c r="C31" s="145"/>
+      <c r="D31" s="57">
+        <f t="shared" ref="D31:AC31" si="2">SUM(D11:D26)</f>
+        <v>8</v>
+      </c>
+      <c r="E31" s="57">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="F31" s="57">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="G31" s="57">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E25" s="57">
-        <f t="shared" si="1"/>
+      <c r="H31" s="57">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F25" s="57">
-        <f t="shared" si="1"/>
+      <c r="I31" s="50">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="J31" s="50">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="K31" s="50">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G25" s="57">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="H25" s="57">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="I25" s="50">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="J25" s="50">
-        <f t="shared" si="1"/>
+      <c r="L31" s="50">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="M31" s="50">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="N31" s="50">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K25" s="50">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="L25" s="50">
-        <f t="shared" si="1"/>
+      <c r="O31" s="50">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M25" s="50">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="N25" s="50">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="O25" s="50">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="P25" s="50">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="Q25" s="50">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="R25" s="50">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="S25" s="50">
-        <f t="shared" si="1"/>
+      <c r="P31" s="50">
+        <f t="shared" si="2"/>
+        <v>1.2</v>
+      </c>
+      <c r="Q31" s="50">
+        <f t="shared" si="2"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="R31" s="50">
+        <f t="shared" si="2"/>
+        <v>2.4</v>
+      </c>
+      <c r="S31" s="50">
+        <f t="shared" si="2"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="T31" s="50">
+        <f t="shared" si="2"/>
+        <v>3.4</v>
+      </c>
+      <c r="U31" s="50">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T25" s="50">
-        <f t="shared" si="1"/>
+      <c r="V31" s="50">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U25" s="50">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="V25" s="50">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="W25" s="50">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="X25" s="50">
-        <f t="shared" si="1"/>
+      <c r="W31" s="50">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y25" s="50">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="Z25" s="50">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="AA25" s="50">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="AB25" s="50">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="AC25" s="50">
-        <v>8</v>
-      </c>
-      <c r="AD25" s="50">
-        <f>SUM(AD11:AD20)</f>
-        <v>8</v>
-      </c>
-      <c r="AE25" s="50">
-        <f>SUM(AE11:AE20)</f>
+      <c r="X31" s="50">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AF25" s="57">
-        <f>SUM(AF11:AF20)</f>
+      <c r="Y31" s="50">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AG25" s="57">
-        <f>SUM(AG11:AG20)</f>
-        <v>8</v>
-      </c>
-      <c r="AH25" s="57">
-        <f>SUM(AH11:AH20)</f>
+      <c r="Z31" s="50">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AI25" s="58">
-        <f>SUM(D25:AH25)</f>
-        <v>163</v>
-      </c>
-      <c r="AJ25" s="73"/>
-    </row>
-    <row r="26" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="27" spans="1:36" s="93" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="91"/>
-      <c r="B27" s="92" t="s">
+      <c r="AA31" s="50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB31" s="50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC31" s="50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AD31" s="50">
+        <f>SUM(AD11:AD26)</f>
+        <v>0</v>
+      </c>
+      <c r="AE31" s="50">
+        <f>SUM(AE11:AE26)</f>
+        <v>0</v>
+      </c>
+      <c r="AF31" s="57">
+        <f>SUM(AF11:AF26)</f>
+        <v>0</v>
+      </c>
+      <c r="AG31" s="57">
+        <f>SUM(AG11:AG26)</f>
+        <v>0</v>
+      </c>
+      <c r="AH31" s="58">
+        <f>SUM(D31:AG31)</f>
+        <v>65.600000000000009</v>
+      </c>
+      <c r="AI31" s="73"/>
+    </row>
+    <row r="32" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="33" spans="1:35" s="93" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="91"/>
+      <c r="B33" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="151"/>
-      <c r="F27" s="151"/>
-      <c r="G27" s="151"/>
-      <c r="H27" s="151"/>
-      <c r="I27" s="151"/>
-      <c r="J27" s="151"/>
-      <c r="S27" s="196" t="s">
+      <c r="D33" s="4"/>
+      <c r="E33" s="152"/>
+      <c r="F33" s="152"/>
+      <c r="G33" s="152"/>
+      <c r="H33" s="152"/>
+      <c r="I33" s="152"/>
+      <c r="J33" s="152"/>
+      <c r="S33" s="197" t="s">
         <v>43</v>
       </c>
-      <c r="T27" s="197"/>
-      <c r="U27" s="197"/>
-      <c r="V27" s="197"/>
-      <c r="W27" s="197"/>
-      <c r="X27" s="197"/>
-      <c r="Y27" s="197"/>
-      <c r="Z27" s="197"/>
-      <c r="AA27" s="198"/>
-      <c r="AC27" s="182" t="s">
+      <c r="T33" s="198"/>
+      <c r="U33" s="198"/>
+      <c r="V33" s="198"/>
+      <c r="W33" s="198"/>
+      <c r="X33" s="198"/>
+      <c r="Y33" s="198"/>
+      <c r="Z33" s="198"/>
+      <c r="AA33" s="199"/>
+      <c r="AC33" s="183" t="s">
         <v>44</v>
       </c>
-      <c r="AD27" s="183"/>
-      <c r="AE27" s="183"/>
-      <c r="AF27" s="183"/>
-      <c r="AG27" s="183"/>
-      <c r="AH27" s="183"/>
-      <c r="AI27" s="183"/>
-      <c r="AJ27" s="184"/>
-    </row>
-    <row r="28" spans="1:36" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="69"/>
-      <c r="B28" s="49" t="s">
+      <c r="AD33" s="184"/>
+      <c r="AE33" s="184"/>
+      <c r="AF33" s="184"/>
+      <c r="AG33" s="184"/>
+      <c r="AH33" s="184"/>
+      <c r="AI33" s="185"/>
+    </row>
+    <row r="34" spans="1:35" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="69"/>
+      <c r="B34" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="151"/>
-      <c r="F28" s="151"/>
-      <c r="G28" s="151"/>
-      <c r="H28" s="151"/>
-      <c r="I28" s="151"/>
-      <c r="J28" s="151"/>
-      <c r="S28" s="185" t="s">
+      <c r="E34" s="152"/>
+      <c r="F34" s="152"/>
+      <c r="G34" s="152"/>
+      <c r="H34" s="152"/>
+      <c r="I34" s="152"/>
+      <c r="J34" s="152"/>
+      <c r="S34" s="186" t="s">
         <v>46</v>
       </c>
-      <c r="T28" s="186"/>
-      <c r="U28" s="187" t="s">
+      <c r="T34" s="187"/>
+      <c r="U34" s="188" t="s">
         <v>47</v>
       </c>
-      <c r="V28" s="187"/>
-      <c r="W28" s="187"/>
-      <c r="X28" s="187"/>
-      <c r="Y28" s="187"/>
-      <c r="Z28" s="187"/>
-      <c r="AA28" s="188"/>
-      <c r="AC28" s="167" t="s">
+      <c r="V34" s="188"/>
+      <c r="W34" s="188"/>
+      <c r="X34" s="188"/>
+      <c r="Y34" s="188"/>
+      <c r="Z34" s="188"/>
+      <c r="AA34" s="189"/>
+      <c r="AC34" s="168" t="s">
         <v>48</v>
       </c>
-      <c r="AD28" s="153"/>
-      <c r="AE28" s="153"/>
-      <c r="AF28" s="153"/>
-      <c r="AG28" s="153"/>
-      <c r="AH28" s="153"/>
-      <c r="AI28" s="153"/>
-      <c r="AJ28" s="154"/>
-    </row>
-    <row r="29" spans="1:36" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="70"/>
-      <c r="B29" s="49" t="s">
+      <c r="AD34" s="154"/>
+      <c r="AE34" s="154"/>
+      <c r="AF34" s="154"/>
+      <c r="AG34" s="154"/>
+      <c r="AH34" s="154"/>
+      <c r="AI34" s="155"/>
+    </row>
+    <row r="35" spans="1:35" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="70"/>
+      <c r="B35" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="E29" s="151"/>
-      <c r="F29" s="151"/>
-      <c r="G29" s="151"/>
-      <c r="H29" s="151"/>
-      <c r="I29" s="151"/>
-      <c r="J29" s="151"/>
-      <c r="S29" s="185"/>
-      <c r="T29" s="186"/>
-      <c r="U29" s="187"/>
-      <c r="V29" s="187"/>
-      <c r="W29" s="187"/>
-      <c r="X29" s="187"/>
-      <c r="Y29" s="187"/>
-      <c r="Z29" s="187"/>
-      <c r="AA29" s="188"/>
-      <c r="AC29" s="168"/>
-      <c r="AD29" s="156"/>
-      <c r="AE29" s="156"/>
-      <c r="AF29" s="156"/>
-      <c r="AG29" s="156"/>
-      <c r="AH29" s="156"/>
-      <c r="AI29" s="156"/>
-      <c r="AJ29" s="157"/>
-    </row>
-    <row r="30" spans="1:36" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="71"/>
-      <c r="B30" s="49" t="s">
+      <c r="E35" s="152"/>
+      <c r="F35" s="152"/>
+      <c r="G35" s="152"/>
+      <c r="H35" s="152"/>
+      <c r="I35" s="152"/>
+      <c r="J35" s="152"/>
+      <c r="S35" s="186"/>
+      <c r="T35" s="187"/>
+      <c r="U35" s="188"/>
+      <c r="V35" s="188"/>
+      <c r="W35" s="188"/>
+      <c r="X35" s="188"/>
+      <c r="Y35" s="188"/>
+      <c r="Z35" s="188"/>
+      <c r="AA35" s="189"/>
+      <c r="AC35" s="169"/>
+      <c r="AD35" s="157"/>
+      <c r="AE35" s="157"/>
+      <c r="AF35" s="157"/>
+      <c r="AG35" s="157"/>
+      <c r="AH35" s="157"/>
+      <c r="AI35" s="158"/>
+    </row>
+    <row r="36" spans="1:35" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="71"/>
+      <c r="B36" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="E30" s="151"/>
-      <c r="F30" s="151"/>
-      <c r="G30" s="151"/>
-      <c r="H30" s="151"/>
-      <c r="I30" s="151"/>
-      <c r="J30" s="151"/>
-      <c r="S30" s="185"/>
-      <c r="T30" s="186"/>
-      <c r="U30" s="187"/>
-      <c r="V30" s="187"/>
-      <c r="W30" s="187"/>
-      <c r="X30" s="187"/>
-      <c r="Y30" s="187"/>
-      <c r="Z30" s="187"/>
-      <c r="AA30" s="188"/>
-      <c r="AC30" s="168"/>
-      <c r="AD30" s="156"/>
-      <c r="AE30" s="156"/>
-      <c r="AF30" s="156"/>
-      <c r="AG30" s="156"/>
-      <c r="AH30" s="156"/>
-      <c r="AI30" s="156"/>
-      <c r="AJ30" s="157"/>
-    </row>
-    <row r="31" spans="1:36" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="S31" s="185"/>
-      <c r="T31" s="186"/>
-      <c r="U31" s="187"/>
-      <c r="V31" s="187"/>
-      <c r="W31" s="187"/>
-      <c r="X31" s="187"/>
-      <c r="Y31" s="187"/>
-      <c r="Z31" s="187"/>
-      <c r="AA31" s="188"/>
-      <c r="AC31" s="168"/>
-      <c r="AD31" s="156"/>
-      <c r="AE31" s="156"/>
-      <c r="AF31" s="156"/>
-      <c r="AG31" s="156"/>
-      <c r="AH31" s="156"/>
-      <c r="AI31" s="156"/>
-      <c r="AJ31" s="157"/>
-    </row>
-    <row r="32" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A32" s="72" t="s">
+      <c r="E36" s="152"/>
+      <c r="F36" s="152"/>
+      <c r="G36" s="152"/>
+      <c r="H36" s="152"/>
+      <c r="I36" s="152"/>
+      <c r="J36" s="152"/>
+      <c r="S36" s="186"/>
+      <c r="T36" s="187"/>
+      <c r="U36" s="188"/>
+      <c r="V36" s="188"/>
+      <c r="W36" s="188"/>
+      <c r="X36" s="188"/>
+      <c r="Y36" s="188"/>
+      <c r="Z36" s="188"/>
+      <c r="AA36" s="189"/>
+      <c r="AC36" s="169"/>
+      <c r="AD36" s="157"/>
+      <c r="AE36" s="157"/>
+      <c r="AF36" s="157"/>
+      <c r="AG36" s="157"/>
+      <c r="AH36" s="157"/>
+      <c r="AI36" s="158"/>
+    </row>
+    <row r="37" spans="1:35" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="S37" s="186"/>
+      <c r="T37" s="187"/>
+      <c r="U37" s="188"/>
+      <c r="V37" s="188"/>
+      <c r="W37" s="188"/>
+      <c r="X37" s="188"/>
+      <c r="Y37" s="188"/>
+      <c r="Z37" s="188"/>
+      <c r="AA37" s="189"/>
+      <c r="AC37" s="169"/>
+      <c r="AD37" s="157"/>
+      <c r="AE37" s="157"/>
+      <c r="AF37" s="157"/>
+      <c r="AG37" s="157"/>
+      <c r="AH37" s="157"/>
+      <c r="AI37" s="158"/>
+    </row>
+    <row r="38" spans="1:35" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A38" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="46"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="44"/>
-      <c r="S32" s="185"/>
-      <c r="T32" s="186"/>
-      <c r="U32" s="187"/>
-      <c r="V32" s="187"/>
-      <c r="W32" s="187"/>
-      <c r="X32" s="187"/>
-      <c r="Y32" s="187"/>
-      <c r="Z32" s="187"/>
-      <c r="AA32" s="188"/>
-      <c r="AC32" s="189"/>
-      <c r="AD32" s="190"/>
-      <c r="AE32" s="190"/>
-      <c r="AF32" s="190"/>
-      <c r="AG32" s="190"/>
-      <c r="AH32" s="190"/>
-      <c r="AI32" s="190"/>
-      <c r="AJ32" s="191"/>
-    </row>
-    <row r="33" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A33" s="148" t="s">
-        <v>52</v>
-      </c>
-      <c r="B33" s="148"/>
-      <c r="C33" s="63">
-        <f>COUNTIF(D24:AH24,"=8")</f>
-        <v>0</v>
-      </c>
-      <c r="D33" s="44"/>
-      <c r="E33" s="44"/>
-      <c r="F33" s="44"/>
-      <c r="G33" s="44"/>
-      <c r="H33" s="44"/>
-      <c r="S33" s="185" t="s">
-        <v>53</v>
-      </c>
-      <c r="T33" s="186"/>
-      <c r="U33" s="187" t="s">
-        <v>54</v>
-      </c>
-      <c r="V33" s="187"/>
-      <c r="W33" s="187"/>
-      <c r="X33" s="187"/>
-      <c r="Y33" s="187"/>
-      <c r="Z33" s="187"/>
-      <c r="AA33" s="188"/>
-      <c r="AC33" s="168" t="s">
-        <v>55</v>
-      </c>
-      <c r="AD33" s="156"/>
-      <c r="AE33" s="156"/>
-      <c r="AF33" s="156"/>
-      <c r="AG33" s="156"/>
-      <c r="AH33" s="156"/>
-      <c r="AI33" s="156"/>
-      <c r="AJ33" s="157"/>
-    </row>
-    <row r="34" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A34" s="63" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" s="47"/>
-      <c r="C34" s="64">
-        <f>NETWORKDAYS(B2,B3)-C33</f>
-        <v>22</v>
-      </c>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="44"/>
-      <c r="H34" s="44"/>
-      <c r="S34" s="185"/>
-      <c r="T34" s="186"/>
-      <c r="U34" s="187"/>
-      <c r="V34" s="187"/>
-      <c r="W34" s="187"/>
-      <c r="X34" s="187"/>
-      <c r="Y34" s="187"/>
-      <c r="Z34" s="187"/>
-      <c r="AA34" s="188"/>
-      <c r="AC34" s="168"/>
-      <c r="AD34" s="156"/>
-      <c r="AE34" s="156"/>
-      <c r="AF34" s="156"/>
-      <c r="AG34" s="156"/>
-      <c r="AH34" s="156"/>
-      <c r="AI34" s="156"/>
-      <c r="AJ34" s="157"/>
-    </row>
-    <row r="35" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A35" s="63" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" s="47"/>
-      <c r="C35" s="63">
-        <f>AI23/8</f>
-        <v>0</v>
-      </c>
-      <c r="D35" s="44"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="44"/>
-      <c r="H35" s="44"/>
-      <c r="S35" s="185"/>
-      <c r="T35" s="186"/>
-      <c r="U35" s="187"/>
-      <c r="V35" s="187"/>
-      <c r="W35" s="187"/>
-      <c r="X35" s="187"/>
-      <c r="Y35" s="187"/>
-      <c r="Z35" s="187"/>
-      <c r="AA35" s="188"/>
-      <c r="AC35" s="168"/>
-      <c r="AD35" s="156"/>
-      <c r="AE35" s="156"/>
-      <c r="AF35" s="156"/>
-      <c r="AG35" s="156"/>
-      <c r="AH35" s="156"/>
-      <c r="AI35" s="156"/>
-      <c r="AJ35" s="157"/>
-    </row>
-    <row r="36" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A36" s="63" t="s">
-        <v>58</v>
-      </c>
-      <c r="B36" s="47"/>
-      <c r="C36" s="63">
-        <f>AI22/8</f>
-        <v>0</v>
-      </c>
-      <c r="D36" s="44"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="44"/>
-      <c r="H36" s="44"/>
-      <c r="S36" s="185"/>
-      <c r="T36" s="186"/>
-      <c r="U36" s="187"/>
-      <c r="V36" s="187"/>
-      <c r="W36" s="187"/>
-      <c r="X36" s="187"/>
-      <c r="Y36" s="187"/>
-      <c r="Z36" s="187"/>
-      <c r="AA36" s="188"/>
-      <c r="AC36" s="168"/>
-      <c r="AD36" s="156"/>
-      <c r="AE36" s="156"/>
-      <c r="AF36" s="156"/>
-      <c r="AG36" s="156"/>
-      <c r="AH36" s="156"/>
-      <c r="AI36" s="156"/>
-      <c r="AJ36" s="157"/>
-    </row>
-    <row r="37" spans="1:36" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="139" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" s="139"/>
-      <c r="C37" s="63">
-        <f>COUNTIF(D25:AH25,"&gt;0")</f>
-        <v>20</v>
-      </c>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="44"/>
-      <c r="H37" s="44"/>
-      <c r="S37" s="192"/>
-      <c r="T37" s="193"/>
-      <c r="U37" s="194"/>
-      <c r="V37" s="194"/>
-      <c r="W37" s="194"/>
-      <c r="X37" s="194"/>
-      <c r="Y37" s="194"/>
-      <c r="Z37" s="194"/>
-      <c r="AA37" s="195"/>
-      <c r="AC37" s="169"/>
-      <c r="AD37" s="159"/>
-      <c r="AE37" s="159"/>
-      <c r="AF37" s="159"/>
-      <c r="AG37" s="159"/>
-      <c r="AH37" s="159"/>
-      <c r="AI37" s="159"/>
-      <c r="AJ37" s="160"/>
-    </row>
-    <row r="38" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A38" s="63" t="s">
-        <v>60</v>
-      </c>
-      <c r="B38" s="47"/>
-      <c r="C38" s="65">
-        <f>C37/(C37+C35+C36)</f>
-        <v>1</v>
-      </c>
+      <c r="B38" s="46"/>
+      <c r="C38" s="63"/>
       <c r="D38" s="44"/>
       <c r="E38" s="44"/>
       <c r="F38" s="44"/>
       <c r="G38" s="44"/>
       <c r="H38" s="44"/>
-    </row>
-    <row r="39" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A39" s="63"/>
-      <c r="B39" s="47"/>
-      <c r="C39" s="63"/>
+      <c r="S38" s="186"/>
+      <c r="T38" s="187"/>
+      <c r="U38" s="188"/>
+      <c r="V38" s="188"/>
+      <c r="W38" s="188"/>
+      <c r="X38" s="188"/>
+      <c r="Y38" s="188"/>
+      <c r="Z38" s="188"/>
+      <c r="AA38" s="189"/>
+      <c r="AC38" s="190"/>
+      <c r="AD38" s="191"/>
+      <c r="AE38" s="191"/>
+      <c r="AF38" s="191"/>
+      <c r="AG38" s="191"/>
+      <c r="AH38" s="191"/>
+      <c r="AI38" s="192"/>
+    </row>
+    <row r="39" spans="1:35" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A39" s="149" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" s="149"/>
+      <c r="C39" s="63">
+        <f>COUNTIF(D30:AG30,"=8")</f>
+        <v>1</v>
+      </c>
       <c r="D39" s="44"/>
       <c r="E39" s="44"/>
       <c r="F39" s="44"/>
       <c r="G39" s="44"/>
       <c r="H39" s="44"/>
-    </row>
-    <row r="40" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A40" s="72" t="s">
-        <v>61</v>
-      </c>
-      <c r="B40" s="46"/>
-      <c r="C40" s="63"/>
+      <c r="S39" s="186" t="s">
+        <v>53</v>
+      </c>
+      <c r="T39" s="187"/>
+      <c r="U39" s="188" t="s">
+        <v>171</v>
+      </c>
+      <c r="V39" s="188"/>
+      <c r="W39" s="188"/>
+      <c r="X39" s="188"/>
+      <c r="Y39" s="188"/>
+      <c r="Z39" s="188"/>
+      <c r="AA39" s="189"/>
+      <c r="AC39" s="169" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD39" s="157"/>
+      <c r="AE39" s="157"/>
+      <c r="AF39" s="157"/>
+      <c r="AG39" s="157"/>
+      <c r="AH39" s="157"/>
+      <c r="AI39" s="158"/>
+    </row>
+    <row r="40" spans="1:35" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A40" s="63" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="47"/>
+      <c r="C40" s="64">
+        <f>NETWORKDAYS(B2,B3)-C39</f>
+        <v>21</v>
+      </c>
       <c r="D40" s="44"/>
       <c r="E40" s="44"/>
       <c r="F40" s="44"/>
       <c r="G40" s="44"/>
       <c r="H40" s="44"/>
-    </row>
-    <row r="41" spans="1:36" ht="35.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="139" t="s">
-        <v>62</v>
-      </c>
-      <c r="B41" s="139"/>
+      <c r="S40" s="186"/>
+      <c r="T40" s="187"/>
+      <c r="U40" s="188"/>
+      <c r="V40" s="188"/>
+      <c r="W40" s="188"/>
+      <c r="X40" s="188"/>
+      <c r="Y40" s="188"/>
+      <c r="Z40" s="188"/>
+      <c r="AA40" s="189"/>
+      <c r="AC40" s="169"/>
+      <c r="AD40" s="157"/>
+      <c r="AE40" s="157"/>
+      <c r="AF40" s="157"/>
+      <c r="AG40" s="157"/>
+      <c r="AH40" s="157"/>
+      <c r="AI40" s="158"/>
+    </row>
+    <row r="41" spans="1:35" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A41" s="63" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" s="47"/>
       <c r="C41" s="63">
-        <f>AI25</f>
-        <v>163</v>
+        <f>AH29/8</f>
+        <v>1</v>
       </c>
       <c r="D41" s="44"/>
       <c r="E41" s="44"/>
       <c r="F41" s="44"/>
       <c r="G41" s="44"/>
       <c r="H41" s="44"/>
-    </row>
-    <row r="42" spans="1:36" ht="38.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="139" t="s">
-        <v>63</v>
-      </c>
-      <c r="B42" s="139"/>
+      <c r="S41" s="186"/>
+      <c r="T41" s="187"/>
+      <c r="U41" s="188"/>
+      <c r="V41" s="188"/>
+      <c r="W41" s="188"/>
+      <c r="X41" s="188"/>
+      <c r="Y41" s="188"/>
+      <c r="Z41" s="188"/>
+      <c r="AA41" s="189"/>
+      <c r="AC41" s="169"/>
+      <c r="AD41" s="157"/>
+      <c r="AE41" s="157"/>
+      <c r="AF41" s="157"/>
+      <c r="AG41" s="157"/>
+      <c r="AH41" s="157"/>
+      <c r="AI41" s="158"/>
+    </row>
+    <row r="42" spans="1:35" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A42" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="47"/>
       <c r="C42" s="63">
-        <v>39</v>
+        <f>AH28/8</f>
+        <v>9</v>
       </c>
       <c r="D42" s="44"/>
       <c r="E42" s="44"/>
       <c r="F42" s="44"/>
       <c r="G42" s="44"/>
       <c r="H42" s="44"/>
-    </row>
-    <row r="43" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A43" s="63" t="s">
-        <v>64</v>
-      </c>
-      <c r="B43" s="48"/>
+      <c r="S42" s="186"/>
+      <c r="T42" s="187"/>
+      <c r="U42" s="188"/>
+      <c r="V42" s="188"/>
+      <c r="W42" s="188"/>
+      <c r="X42" s="188"/>
+      <c r="Y42" s="188"/>
+      <c r="Z42" s="188"/>
+      <c r="AA42" s="189"/>
+      <c r="AC42" s="169"/>
+      <c r="AD42" s="157"/>
+      <c r="AE42" s="157"/>
+      <c r="AF42" s="157"/>
+      <c r="AG42" s="157"/>
+      <c r="AH42" s="157"/>
+      <c r="AI42" s="158"/>
+    </row>
+    <row r="43" spans="1:35" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A43" s="140" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="140"/>
       <c r="C43" s="63">
-        <f>SUMIFS($AI$12:$AI$20, $C$12:$C$20, "Morning")</f>
-        <v>25</v>
+        <f>COUNTIF(D31:AG31,"&gt;0")</f>
+        <v>12</v>
       </c>
       <c r="D43" s="44"/>
       <c r="E43" s="44"/>
       <c r="F43" s="44"/>
       <c r="G43" s="44"/>
       <c r="H43" s="44"/>
-    </row>
-    <row r="44" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="S43" s="193"/>
+      <c r="T43" s="194"/>
+      <c r="U43" s="195"/>
+      <c r="V43" s="195"/>
+      <c r="W43" s="195"/>
+      <c r="X43" s="195"/>
+      <c r="Y43" s="195"/>
+      <c r="Z43" s="195"/>
+      <c r="AA43" s="196"/>
+      <c r="AC43" s="170"/>
+      <c r="AD43" s="160"/>
+      <c r="AE43" s="160"/>
+      <c r="AF43" s="160"/>
+      <c r="AG43" s="160"/>
+      <c r="AH43" s="160"/>
+      <c r="AI43" s="161"/>
+    </row>
+    <row r="44" spans="1:35" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A44" s="63" t="s">
-        <v>65</v>
-      </c>
-      <c r="B44" s="48"/>
-      <c r="C44" s="63">
-        <f>SUMIFS($AI$12:$AI$20, $C$12:$C$20, "Afternoon")</f>
-        <v>7</v>
+        <v>60</v>
+      </c>
+      <c r="B44" s="47"/>
+      <c r="C44" s="65">
+        <f>C43/(C43+C41+C42)</f>
+        <v>0.54545454545454541</v>
       </c>
       <c r="D44" s="44"/>
       <c r="E44" s="44"/>
       <c r="F44" s="44"/>
       <c r="G44" s="44"/>
       <c r="H44" s="44"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="44"/>
-    </row>
-    <row r="45" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A45" s="63" t="s">
-        <v>66</v>
-      </c>
-      <c r="B45" s="48"/>
-      <c r="C45" s="63">
-        <f>SUMIFS($AI$12:$AI$20, $C$12:$C$20, "Night")</f>
-        <v>18</v>
-      </c>
+    </row>
+    <row r="45" spans="1:35" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A45" s="63"/>
+      <c r="B45" s="47"/>
+      <c r="C45" s="63"/>
       <c r="D45" s="44"/>
       <c r="E45" s="44"/>
       <c r="F45" s="44"/>
       <c r="G45" s="44"/>
       <c r="H45" s="44"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="44"/>
-    </row>
-    <row r="46" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A46" s="63"/>
-      <c r="B46" s="47"/>
+    </row>
+    <row r="46" spans="1:35" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A46" s="72" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46" s="46"/>
       <c r="C46" s="63"/>
       <c r="D46" s="44"/>
       <c r="E46" s="44"/>
       <c r="F46" s="44"/>
       <c r="G46" s="44"/>
       <c r="H46" s="44"/>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
-    </row>
-    <row r="47" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A47" s="72" t="s">
-        <v>67</v>
-      </c>
-      <c r="B47" s="46"/>
-      <c r="C47" s="63"/>
+    </row>
+    <row r="47" spans="1:35" ht="35.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="140" t="s">
+        <v>62</v>
+      </c>
+      <c r="B47" s="140"/>
+      <c r="C47" s="63">
+        <f>AH31</f>
+        <v>65.600000000000009</v>
+      </c>
       <c r="D47" s="44"/>
       <c r="E47" s="44"/>
       <c r="F47" s="44"/>
       <c r="G47" s="44"/>
       <c r="H47" s="44"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
-    </row>
-    <row r="48" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A48" s="63" t="s">
-        <v>68</v>
-      </c>
-      <c r="B48" s="47"/>
-      <c r="C48" s="63"/>
+    </row>
+    <row r="48" spans="1:35" ht="38.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="140" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" s="140"/>
+      <c r="C48" s="63">
+        <v>39</v>
+      </c>
       <c r="D48" s="44"/>
       <c r="E48" s="44"/>
       <c r="F48" s="44"/>
       <c r="G48" s="44"/>
       <c r="H48" s="44"/>
-      <c r="I48" s="44"/>
-      <c r="J48" s="44"/>
     </row>
     <row r="49" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A49" s="63" t="s">
-        <v>69</v>
-      </c>
-      <c r="B49" s="47"/>
-      <c r="C49" s="63"/>
+        <v>64</v>
+      </c>
+      <c r="B49" s="48"/>
+      <c r="C49" s="63">
+        <f>SUMIFS($AH$12:$AH$26, $C$12:$C$26, "Morning")</f>
+        <v>11</v>
+      </c>
       <c r="D49" s="44"/>
       <c r="E49" s="44"/>
       <c r="F49" s="44"/>
       <c r="G49" s="44"/>
       <c r="H49" s="44"/>
-      <c r="I49" s="44"/>
-      <c r="J49" s="44"/>
     </row>
     <row r="50" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A50" s="63"/>
-      <c r="B50" s="47"/>
-      <c r="C50" s="63"/>
+      <c r="A50" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" s="48"/>
+      <c r="C50" s="63">
+        <f>SUMIFS($AH$12:$AH$26, $C$12:$C$26, "Afternoon")</f>
+        <v>3</v>
+      </c>
       <c r="D50" s="44"/>
       <c r="E50" s="44"/>
       <c r="F50" s="44"/>
@@ -6320,28 +6533,112 @@
       <c r="I50" s="44"/>
       <c r="J50" s="44"/>
     </row>
-    <row r="52" spans="1:10" ht="155.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="53" spans="1:10" ht="169" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="51" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A51" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" s="48"/>
+      <c r="C51" s="63">
+        <f>SUMIFS($AH$12:$AH$26, $C$12:$C$26, "Night")</f>
+        <v>0</v>
+      </c>
+      <c r="D51" s="44"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="44"/>
+      <c r="G51" s="44"/>
+      <c r="H51" s="44"/>
+      <c r="I51" s="44"/>
+      <c r="J51" s="44"/>
+    </row>
+    <row r="52" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A52" s="63"/>
+      <c r="B52" s="47"/>
+      <c r="C52" s="63"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
+      <c r="G52" s="44"/>
+      <c r="H52" s="44"/>
+      <c r="I52" s="44"/>
+      <c r="J52" s="44"/>
+    </row>
+    <row r="53" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A53" s="72" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" s="46"/>
+      <c r="C53" s="63"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="44"/>
+      <c r="G53" s="44"/>
+      <c r="H53" s="44"/>
+      <c r="I53" s="44"/>
+      <c r="J53" s="44"/>
+    </row>
+    <row r="54" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A54" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" s="47"/>
+      <c r="C54" s="63"/>
+      <c r="D54" s="44"/>
+      <c r="E54" s="44"/>
+      <c r="F54" s="44"/>
+      <c r="G54" s="44"/>
+      <c r="H54" s="44"/>
+      <c r="I54" s="44"/>
+      <c r="J54" s="44"/>
+    </row>
+    <row r="55" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A55" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="B55" s="47"/>
+      <c r="C55" s="63"/>
+      <c r="D55" s="44"/>
+      <c r="E55" s="44"/>
+      <c r="F55" s="44"/>
+      <c r="G55" s="44"/>
+      <c r="H55" s="44"/>
+      <c r="I55" s="44"/>
+      <c r="J55" s="44"/>
+    </row>
+    <row r="56" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A56" s="63"/>
+      <c r="B56" s="47"/>
+      <c r="C56" s="63"/>
+      <c r="D56" s="44"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="44"/>
+      <c r="G56" s="44"/>
+      <c r="H56" s="44"/>
+      <c r="I56" s="44"/>
+      <c r="J56" s="44"/>
+    </row>
+    <row r="58" spans="1:10" ht="155.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="59" spans="1:10" ht="169" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="AC27:AJ27"/>
-    <mergeCell ref="S28:T32"/>
-    <mergeCell ref="U28:AA32"/>
-    <mergeCell ref="AC28:AJ32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="S33:T37"/>
-    <mergeCell ref="U33:AA37"/>
-    <mergeCell ref="AC33:AJ37"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="S27:AA27"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="E27:J30"/>
-    <mergeCell ref="AI9:AI10"/>
+  <mergeCells count="24">
+    <mergeCell ref="A12:A21"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="AC33:AI33"/>
+    <mergeCell ref="S34:T38"/>
+    <mergeCell ref="U34:AA38"/>
+    <mergeCell ref="AC34:AI38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="S39:T43"/>
+    <mergeCell ref="U39:AA43"/>
+    <mergeCell ref="AC39:AI43"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="S33:AA33"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="E33:J36"/>
+    <mergeCell ref="AH9:AH10"/>
     <mergeCell ref="N5:Q5"/>
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="A9:A10"/>
@@ -6358,20 +6655,20 @@
       <formula>TEXT(B3,"mmm")&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D9:AH20 D21:AF21 D22:AH25">
-    <cfRule type="expression" dxfId="3" priority="3">
+  <conditionalFormatting sqref="D31:AG31">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="lessThan">
+      <formula>8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9:AG26 D27:AF27 D28:AG31">
+    <cfRule type="expression" dxfId="1" priority="33">
       <formula>OR(D$9="Sat",D$9="Sun")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>D$24=8</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D25:AH25">
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="greaterThan">
-      <formula>8</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="lessThan">
-      <formula>8</formula>
+    <cfRule type="expression" dxfId="0" priority="34">
+      <formula>D$30=8</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -6390,7 +6687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B05E5B8-DD91-4132-B819-9B05D1BA41C5}">
   <dimension ref="A1:Z67"/>
   <sheetViews>
-    <sheetView zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -6437,7 +6734,7 @@
       <c r="B2" s="5"/>
       <c r="C2" s="94"/>
       <c r="D2" s="99" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="99"/>
@@ -6495,7 +6792,7 @@
       <c r="B4" s="5"/>
       <c r="C4" s="94"/>
       <c r="D4" s="100" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="100"/>
@@ -6578,11 +6875,11 @@
     </row>
     <row r="7" spans="1:26" ht="26.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C7" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D7" s="36"/>
       <c r="E7" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="12"/>
@@ -6591,7 +6888,7 @@
       <c r="C8" s="10"/>
       <c r="D8" s="37"/>
       <c r="E8" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="12"/>
@@ -6605,27 +6902,27 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B10" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="95" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="95" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="95" t="s">
+      <c r="E10" s="101" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="95" t="s">
+      <c r="F10" s="95" t="s">
         <v>79</v>
       </c>
-      <c r="E10" s="101" t="s">
+      <c r="G10" s="13" t="s">
         <v>80</v>
-      </c>
-      <c r="F10" s="95" t="s">
-        <v>81</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="38" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C11" s="96"/>
       <c r="D11" s="96"/>
@@ -6641,16 +6938,16 @@
         <v>0</v>
       </c>
       <c r="D12" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="G12" s="17" t="s">
         <v>85</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="26" x14ac:dyDescent="0.35">
@@ -6661,16 +6958,16 @@
         <v>6</v>
       </c>
       <c r="D13" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="19" t="s">
         <v>88</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>90</v>
       </c>
       <c r="H13" s="3"/>
     </row>
@@ -6679,19 +6976,19 @@
         <v>3</v>
       </c>
       <c r="C14" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="G14" s="19" t="s">
         <v>92</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>94</v>
       </c>
       <c r="H14" s="23"/>
     </row>
@@ -6703,16 +7000,16 @@
         <v>18</v>
       </c>
       <c r="D15" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="G15" s="19" t="s">
         <v>95</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>97</v>
       </c>
       <c r="H15" s="23"/>
     </row>
@@ -6724,16 +7021,16 @@
         <v>8</v>
       </c>
       <c r="D16" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" s="19" t="s">
         <v>98</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>100</v>
       </c>
       <c r="H16" s="23"/>
     </row>
@@ -6745,16 +7042,16 @@
         <v>14</v>
       </c>
       <c r="D17" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="G17" s="19" t="s">
         <v>101</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="G17" s="19" t="s">
-        <v>103</v>
       </c>
       <c r="H17" s="23"/>
     </row>
@@ -6763,19 +7060,19 @@
         <v>7</v>
       </c>
       <c r="C18" s="138" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="G18" s="19" t="s">
         <v>105</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="G18" s="19" t="s">
-        <v>107</v>
       </c>
       <c r="H18" s="23"/>
     </row>
@@ -6784,25 +7081,25 @@
         <v>8</v>
       </c>
       <c r="C19" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="G19" s="21" t="s">
         <v>109</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="G19" s="21" t="s">
-        <v>111</v>
       </c>
       <c r="H19" s="24"/>
     </row>
     <row r="20" spans="2:8" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C20" s="96"/>
       <c r="D20" s="96"/>
@@ -6816,19 +7113,19 @@
         <v>9</v>
       </c>
       <c r="C21" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="G21" s="19" t="s">
         <v>114</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="G21" s="19" t="s">
-        <v>116</v>
       </c>
       <c r="H21" s="24"/>
     </row>
@@ -6840,16 +7137,16 @@
         <v>21</v>
       </c>
       <c r="D22" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="G22" s="25" t="s">
         <v>117</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="F22" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="G22" s="25" t="s">
-        <v>119</v>
       </c>
       <c r="H22" s="24"/>
     </row>
@@ -6858,19 +7155,19 @@
         <v>11</v>
       </c>
       <c r="C23" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F23" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="G23" s="19" t="s">
         <v>121</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="F23" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="G23" s="19" t="s">
-        <v>123</v>
       </c>
       <c r="H23" s="1"/>
     </row>
@@ -6879,19 +7176,19 @@
         <v>12</v>
       </c>
       <c r="C24" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="E24" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="F24" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="G24" s="19" t="s">
         <v>126</v>
-      </c>
-      <c r="F24" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="G24" s="19" t="s">
-        <v>128</v>
       </c>
       <c r="H24" s="24"/>
     </row>
@@ -6900,19 +7197,19 @@
         <v>13</v>
       </c>
       <c r="C25" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="F25" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="D25" s="26" t="s">
+      <c r="G25" s="19" t="s">
         <v>130</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="F25" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="G25" s="19" t="s">
-        <v>132</v>
       </c>
       <c r="H25" s="1"/>
     </row>
@@ -6921,23 +7218,23 @@
         <v>14</v>
       </c>
       <c r="C26" s="103" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F26" s="27"/>
       <c r="G26" s="30" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="2:8" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="104" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C27" s="105"/>
       <c r="D27" s="105"/>
@@ -6954,10 +7251,10 @@
         <v>52</v>
       </c>
       <c r="D28" s="109" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F28" s="110"/>
       <c r="G28" s="111"/>
@@ -6971,10 +7268,10 @@
         <v>56</v>
       </c>
       <c r="D29" s="109" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F29" s="113"/>
       <c r="G29" s="114"/>
@@ -6988,10 +7285,10 @@
         <v>57</v>
       </c>
       <c r="D30" s="109" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F30" s="113"/>
       <c r="G30" s="114"/>
@@ -7005,10 +7302,10 @@
         <v>58</v>
       </c>
       <c r="D31" s="109" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F31" s="113"/>
       <c r="G31" s="114"/>
@@ -7022,10 +7319,10 @@
         <v>59</v>
       </c>
       <c r="D32" s="109" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F32" s="113"/>
       <c r="G32" s="114"/>
@@ -7039,10 +7336,10 @@
         <v>60</v>
       </c>
       <c r="D33" s="109" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E33" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F33" s="113"/>
       <c r="G33" s="114"/>
@@ -7056,10 +7353,10 @@
         <v>62</v>
       </c>
       <c r="D34" s="109" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F34" s="113"/>
       <c r="G34" s="114"/>
@@ -7070,19 +7367,19 @@
         <v>22</v>
       </c>
       <c r="C35" s="116" t="s">
+        <v>143</v>
+      </c>
+      <c r="D35" s="117" t="s">
+        <v>144</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="F35" s="118" t="s">
         <v>145</v>
       </c>
-      <c r="D35" s="117" t="s">
+      <c r="G35" s="119" t="s">
         <v>146</v>
-      </c>
-      <c r="E35" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="F35" s="118" t="s">
-        <v>147</v>
-      </c>
-      <c r="G35" s="119" t="s">
-        <v>148</v>
       </c>
       <c r="H35" s="24"/>
     </row>
@@ -7094,10 +7391,10 @@
         <v>64</v>
       </c>
       <c r="D36" s="121" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F36" s="113"/>
       <c r="G36" s="114"/>
@@ -7111,10 +7408,10 @@
         <v>65</v>
       </c>
       <c r="D37" s="121" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F37" s="113"/>
       <c r="G37" s="114"/>
@@ -7128,10 +7425,10 @@
         <v>66</v>
       </c>
       <c r="D38" s="121" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F38" s="113"/>
       <c r="G38" s="114"/>
@@ -7142,17 +7439,17 @@
         <v>26</v>
       </c>
       <c r="C39" s="115" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D39" s="122" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E39" s="122" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F39" s="121"/>
       <c r="G39" s="121" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H39" s="24"/>
     </row>
@@ -7161,19 +7458,19 @@
         <v>27</v>
       </c>
       <c r="C40" s="115" t="s">
+        <v>153</v>
+      </c>
+      <c r="D40" s="122" t="s">
+        <v>154</v>
+      </c>
+      <c r="E40" s="119" t="s">
         <v>155</v>
       </c>
-      <c r="D40" s="122" t="s">
+      <c r="F40" s="122" t="s">
         <v>156</v>
       </c>
-      <c r="E40" s="119" t="s">
+      <c r="G40" s="119" t="s">
         <v>157</v>
-      </c>
-      <c r="F40" s="122" t="s">
-        <v>158</v>
-      </c>
-      <c r="G40" s="119" t="s">
-        <v>159</v>
       </c>
       <c r="H40" s="24"/>
     </row>
@@ -7182,19 +7479,19 @@
         <v>28</v>
       </c>
       <c r="C41" s="115" t="s">
+        <v>158</v>
+      </c>
+      <c r="D41" s="122" t="s">
+        <v>159</v>
+      </c>
+      <c r="E41" s="119" t="s">
         <v>160</v>
       </c>
-      <c r="D41" s="122" t="s">
+      <c r="F41" s="122" t="s">
         <v>161</v>
       </c>
-      <c r="E41" s="119" t="s">
+      <c r="G41" s="119" t="s">
         <v>162</v>
-      </c>
-      <c r="F41" s="122" t="s">
-        <v>163</v>
-      </c>
-      <c r="G41" s="119" t="s">
-        <v>164</v>
       </c>
       <c r="H41" s="24"/>
     </row>
@@ -7244,7 +7541,7 @@
       <c r="C47" s="129"/>
       <c r="D47" s="122"/>
       <c r="E47" s="119"/>
-      <c r="F47" s="199"/>
+      <c r="F47" s="200"/>
       <c r="G47" s="122"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.35">
@@ -7252,7 +7549,7 @@
       <c r="C48" s="128"/>
       <c r="D48" s="122"/>
       <c r="E48" s="119"/>
-      <c r="F48" s="199"/>
+      <c r="F48" s="200"/>
       <c r="G48" s="122"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.35">
@@ -7260,7 +7557,7 @@
       <c r="C49" s="128"/>
       <c r="D49" s="122"/>
       <c r="E49" s="119"/>
-      <c r="F49" s="199"/>
+      <c r="F49" s="200"/>
       <c r="G49" s="122"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.35">
@@ -7268,7 +7565,7 @@
       <c r="C50" s="129"/>
       <c r="D50" s="122"/>
       <c r="E50" s="119"/>
-      <c r="F50" s="199"/>
+      <c r="F50" s="200"/>
       <c r="G50" s="122"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.35">
@@ -7428,6 +7725,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CBBA4E8384962545BF977EF5EB207524" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4c71af4b5276cc520d7caa7153b08011">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ecef1726-c816-4ce0-a2de-c7222e5e0303" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d40dcfb130600d1adddbff1088e0e0d5" ns2:_="">
     <xsd:import namespace="ecef1726-c816-4ce0-a2de-c7222e5e0303"/>
@@ -7571,16 +7877,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39A50F55-EB9E-48CA-A399-9CBC9253A5CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E1BDC32-896F-448F-9DE0-A2D567D26AC8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7596,12 +7901,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39A50F55-EB9E-48CA-A399-9CBC9253A5CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>